<commit_message>
Files cleaning - Physical Activity
</commit_message>
<xml_diff>
--- a/2003/Adul03.xlsx
+++ b/2003/Adul03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidaddealcala-my.sharepoint.com/personal/pedro_gullon_uah_es/Documents/FIS 2021/dta/cvd_inequities_spain/2003/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidaddealcala-my.sharepoint.com/personal/luis_cereijo_uah_es/Documents/Investigacion/FIS_CVDinequities/R/cvd_inequities_spain/2003/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{58829393-899F-4209-936B-591AFA539018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20371880-55D3-4642-B7F8-27D391302AAE}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{58829393-899F-4209-936B-591AFA539018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9D1E98F-AB6B-4509-BC88-59080051129C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -13951,32 +13951,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="15"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="15"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14298,14 +14298,14 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.35546875" defaultRowHeight="13.15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="11.5"/>
-    <col min="3" max="4" width="15.1640625" customWidth="1"/>
-    <col min="5" max="5" width="43.33203125" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" customWidth="1"/>
-    <col min="7" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="3" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="43.35546875" customWidth="1"/>
+    <col min="6" max="6" width="4.640625" customWidth="1"/>
+    <col min="7" max="1025" width="8.640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24.4" customHeight="1">
@@ -20019,24 +20019,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F420"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A414" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A419" sqref="A419:F419"/>
+    <sheetView tabSelected="1" topLeftCell="A406" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A416" sqref="A416:F416"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.35546875" defaultRowHeight="13.15"/>
   <cols>
-    <col min="1" max="1025" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1025" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="48.75" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="62.25" customHeight="1">
       <c r="A2" s="13" t="s">
@@ -20079,14 +20079,14 @@
       <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" ht="76.5" customHeight="1">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="14" t="s">
         <v>350</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" ht="55.5" customHeight="1">
       <c r="A7" s="13" t="s">
@@ -20609,14 +20609,14 @@
       <c r="F58" s="15"/>
     </row>
     <row r="59" spans="1:6" ht="33" customHeight="1">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
     </row>
     <row r="60" spans="1:6" ht="34.5" customHeight="1">
       <c r="A60" s="15" t="s">
@@ -20629,14 +20629,14 @@
       <c r="F60" s="15"/>
     </row>
     <row r="61" spans="1:6" ht="33" customHeight="1">
-      <c r="A61" s="12" t="s">
+      <c r="A61" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
     </row>
     <row r="62" spans="1:6" ht="34.5" customHeight="1">
       <c r="A62" s="15" t="s">
@@ -20649,14 +20649,14 @@
       <c r="F62" s="15"/>
     </row>
     <row r="63" spans="1:6" ht="33" customHeight="1">
-      <c r="A63" s="12" t="s">
+      <c r="A63" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
     </row>
     <row r="64" spans="1:6" ht="55.5" customHeight="1">
       <c r="A64" s="13" t="s">
@@ -20689,14 +20689,14 @@
       <c r="F66" s="13"/>
     </row>
     <row r="67" spans="1:6" ht="33" customHeight="1">
-      <c r="A67" s="12" t="s">
+      <c r="A67" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
     </row>
     <row r="68" spans="1:6" ht="34.5" customHeight="1">
       <c r="A68" s="15" t="s">
@@ -20709,14 +20709,14 @@
       <c r="F68" s="15"/>
     </row>
     <row r="69" spans="1:6" ht="33" customHeight="1">
-      <c r="A69" s="12" t="s">
+      <c r="A69" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
     </row>
     <row r="70" spans="1:6" ht="55.5" customHeight="1">
       <c r="A70" s="15" t="s">
@@ -20739,14 +20739,14 @@
       <c r="F71" s="15"/>
     </row>
     <row r="72" spans="1:6" ht="33" customHeight="1">
-      <c r="A72" s="12" t="s">
+      <c r="A72" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
     </row>
     <row r="73" spans="1:6" ht="55.5" customHeight="1">
       <c r="A73" s="15" t="s">
@@ -20789,24 +20789,24 @@
       <c r="F76" s="15"/>
     </row>
     <row r="77" spans="1:6" ht="66" customHeight="1">
-      <c r="A77" s="18" t="s">
+      <c r="A77" s="17" t="s">
         <v>416</v>
       </c>
-      <c r="B77" s="18"/>
-      <c r="C77" s="18"/>
-      <c r="D77" s="18"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="18"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
     </row>
     <row r="78" spans="1:6" ht="33" customHeight="1">
-      <c r="A78" s="12" t="s">
+      <c r="A78" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="16"/>
+      <c r="F78" s="16"/>
     </row>
     <row r="79" spans="1:6" ht="34.5" customHeight="1">
       <c r="A79" s="15" t="s">
@@ -20819,14 +20819,14 @@
       <c r="F79" s="15"/>
     </row>
     <row r="80" spans="1:6" ht="33" customHeight="1">
-      <c r="A80" s="12" t="s">
+      <c r="A80" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B80" s="12"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
     </row>
     <row r="81" spans="1:6" ht="34.5" customHeight="1">
       <c r="A81" s="15" t="s">
@@ -20839,14 +20839,14 @@
       <c r="F81" s="15"/>
     </row>
     <row r="82" spans="1:6" ht="33" customHeight="1">
-      <c r="A82" s="12" t="s">
+      <c r="A82" s="16" t="s">
         <v>419</v>
       </c>
-      <c r="B82" s="12"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="16"/>
     </row>
     <row r="83" spans="1:6" ht="34.5" customHeight="1">
       <c r="A83" s="15" t="s">
@@ -20859,14 +20859,14 @@
       <c r="F83" s="15"/>
     </row>
     <row r="84" spans="1:6" ht="33" customHeight="1">
-      <c r="A84" s="12" t="s">
+      <c r="A84" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B84" s="12"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
     </row>
     <row r="85" spans="1:6" ht="34.5" customHeight="1">
       <c r="A85" s="15" t="s">
@@ -20879,14 +20879,14 @@
       <c r="F85" s="15"/>
     </row>
     <row r="86" spans="1:6" ht="33" customHeight="1">
-      <c r="A86" s="12" t="s">
+      <c r="A86" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B86" s="12"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="16"/>
+      <c r="E86" s="16"/>
+      <c r="F86" s="16"/>
     </row>
     <row r="87" spans="1:6" ht="34.5" customHeight="1">
       <c r="A87" s="15" t="s">
@@ -20899,34 +20899,34 @@
       <c r="F87" s="15"/>
     </row>
     <row r="88" spans="1:6" ht="33" customHeight="1">
-      <c r="A88" s="12" t="s">
+      <c r="A88" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B88" s="12"/>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="12"/>
+      <c r="B88" s="16"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="16"/>
+      <c r="E88" s="16"/>
+      <c r="F88" s="16"/>
     </row>
     <row r="89" spans="1:6" ht="34.5" customHeight="1">
-      <c r="A89" s="17" t="s">
+      <c r="A89" s="18" t="s">
         <v>423</v>
       </c>
-      <c r="B89" s="17"/>
-      <c r="C89" s="17"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
     </row>
     <row r="90" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A90" s="12" t="s">
+      <c r="A90" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12"/>
+      <c r="B90" s="16"/>
+      <c r="C90" s="16"/>
+      <c r="D90" s="16"/>
+      <c r="E90" s="16"/>
+      <c r="F90" s="16"/>
     </row>
     <row r="91" spans="1:6" ht="55.5" customHeight="1">
       <c r="A91" s="13" t="s">
@@ -20959,14 +20959,14 @@
       <c r="F93" s="13"/>
     </row>
     <row r="94" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A94" s="12" t="s">
+      <c r="A94" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B94" s="12"/>
-      <c r="C94" s="12"/>
-      <c r="D94" s="12"/>
-      <c r="E94" s="12"/>
-      <c r="F94" s="12"/>
+      <c r="B94" s="16"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="16"/>
+      <c r="E94" s="16"/>
+      <c r="F94" s="16"/>
     </row>
     <row r="95" spans="1:6" ht="34.5" customHeight="1">
       <c r="A95" s="13" t="s">
@@ -20979,14 +20979,14 @@
       <c r="F95" s="13"/>
     </row>
     <row r="96" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A96" s="12" t="s">
+      <c r="A96" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B96" s="12"/>
-      <c r="C96" s="12"/>
-      <c r="D96" s="12"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="12"/>
+      <c r="B96" s="16"/>
+      <c r="C96" s="16"/>
+      <c r="D96" s="16"/>
+      <c r="E96" s="16"/>
+      <c r="F96" s="16"/>
     </row>
     <row r="97" spans="1:6" ht="34.5" customHeight="1">
       <c r="A97" s="13" t="s">
@@ -20999,14 +20999,14 @@
       <c r="F97" s="13"/>
     </row>
     <row r="98" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A98" s="12" t="s">
+      <c r="A98" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B98" s="12"/>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12"/>
+      <c r="B98" s="16"/>
+      <c r="C98" s="16"/>
+      <c r="D98" s="16"/>
+      <c r="E98" s="16"/>
+      <c r="F98" s="16"/>
     </row>
     <row r="99" spans="1:6" ht="34.5" customHeight="1">
       <c r="A99" s="13" t="s">
@@ -21019,14 +21019,14 @@
       <c r="F99" s="13"/>
     </row>
     <row r="100" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A100" s="12" t="s">
+      <c r="A100" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B100" s="12"/>
-      <c r="C100" s="12"/>
-      <c r="D100" s="12"/>
-      <c r="E100" s="12"/>
-      <c r="F100" s="12"/>
+      <c r="B100" s="16"/>
+      <c r="C100" s="16"/>
+      <c r="D100" s="16"/>
+      <c r="E100" s="16"/>
+      <c r="F100" s="16"/>
     </row>
     <row r="101" spans="1:6" ht="34.5" customHeight="1">
       <c r="A101" s="13" t="s">
@@ -21039,14 +21039,14 @@
       <c r="F101" s="13"/>
     </row>
     <row r="102" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A102" s="12" t="s">
+      <c r="A102" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B102" s="12"/>
-      <c r="C102" s="12"/>
-      <c r="D102" s="12"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
+      <c r="B102" s="16"/>
+      <c r="C102" s="16"/>
+      <c r="D102" s="16"/>
+      <c r="E102" s="16"/>
+      <c r="F102" s="16"/>
     </row>
     <row r="103" spans="1:6" ht="34.5" customHeight="1">
       <c r="A103" s="13" t="s">
@@ -21059,14 +21059,14 @@
       <c r="F103" s="13"/>
     </row>
     <row r="104" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A104" s="12" t="s">
+      <c r="A104" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B104" s="12"/>
-      <c r="C104" s="12"/>
-      <c r="D104" s="12"/>
-      <c r="E104" s="12"/>
-      <c r="F104" s="12"/>
+      <c r="B104" s="16"/>
+      <c r="C104" s="16"/>
+      <c r="D104" s="16"/>
+      <c r="E104" s="16"/>
+      <c r="F104" s="16"/>
     </row>
     <row r="105" spans="1:6" ht="66" customHeight="1">
       <c r="A105" s="13" t="s">
@@ -21089,14 +21089,14 @@
       <c r="F106" s="13"/>
     </row>
     <row r="107" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A107" s="12" t="s">
+      <c r="A107" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B107" s="12"/>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
-      <c r="E107" s="12"/>
-      <c r="F107" s="12"/>
+      <c r="B107" s="16"/>
+      <c r="C107" s="16"/>
+      <c r="D107" s="16"/>
+      <c r="E107" s="16"/>
+      <c r="F107" s="16"/>
     </row>
     <row r="108" spans="1:6" ht="34.5" customHeight="1">
       <c r="A108" s="13" t="s">
@@ -21109,14 +21109,14 @@
       <c r="F108" s="13"/>
     </row>
     <row r="109" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A109" s="12" t="s">
+      <c r="A109" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B109" s="12"/>
-      <c r="C109" s="12"/>
-      <c r="D109" s="12"/>
-      <c r="E109" s="12"/>
-      <c r="F109" s="12"/>
+      <c r="B109" s="16"/>
+      <c r="C109" s="16"/>
+      <c r="D109" s="16"/>
+      <c r="E109" s="16"/>
+      <c r="F109" s="16"/>
     </row>
     <row r="110" spans="1:6" ht="34.5" customHeight="1">
       <c r="A110" s="13" t="s">
@@ -21129,14 +21129,14 @@
       <c r="F110" s="13"/>
     </row>
     <row r="111" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A111" s="12" t="s">
+      <c r="A111" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B111" s="12"/>
-      <c r="C111" s="12"/>
-      <c r="D111" s="12"/>
-      <c r="E111" s="12"/>
-      <c r="F111" s="12"/>
+      <c r="B111" s="16"/>
+      <c r="C111" s="16"/>
+      <c r="D111" s="16"/>
+      <c r="E111" s="16"/>
+      <c r="F111" s="16"/>
     </row>
     <row r="112" spans="1:6" ht="34.5" customHeight="1">
       <c r="A112" s="13" t="s">
@@ -21149,14 +21149,14 @@
       <c r="F112" s="13"/>
     </row>
     <row r="113" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A113" s="12" t="s">
+      <c r="A113" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B113" s="12"/>
-      <c r="C113" s="12"/>
-      <c r="D113" s="12"/>
-      <c r="E113" s="12"/>
-      <c r="F113" s="12"/>
+      <c r="B113" s="16"/>
+      <c r="C113" s="16"/>
+      <c r="D113" s="16"/>
+      <c r="E113" s="16"/>
+      <c r="F113" s="16"/>
     </row>
     <row r="114" spans="1:6" ht="34.5" customHeight="1">
       <c r="A114" s="13" t="s">
@@ -21169,14 +21169,14 @@
       <c r="F114" s="13"/>
     </row>
     <row r="115" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A115" s="12" t="s">
+      <c r="A115" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B115" s="12"/>
-      <c r="C115" s="12"/>
-      <c r="D115" s="12"/>
-      <c r="E115" s="12"/>
-      <c r="F115" s="12"/>
+      <c r="B115" s="16"/>
+      <c r="C115" s="16"/>
+      <c r="D115" s="16"/>
+      <c r="E115" s="16"/>
+      <c r="F115" s="16"/>
     </row>
     <row r="116" spans="1:6" ht="34.5" customHeight="1">
       <c r="A116" s="13" t="s">
@@ -21189,14 +21189,14 @@
       <c r="F116" s="13"/>
     </row>
     <row r="117" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A117" s="12" t="s">
+      <c r="A117" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B117" s="12"/>
-      <c r="C117" s="12"/>
-      <c r="D117" s="12"/>
-      <c r="E117" s="12"/>
-      <c r="F117" s="12"/>
+      <c r="B117" s="16"/>
+      <c r="C117" s="16"/>
+      <c r="D117" s="16"/>
+      <c r="E117" s="16"/>
+      <c r="F117" s="16"/>
     </row>
     <row r="118" spans="1:6" ht="34.5" customHeight="1">
       <c r="A118" s="13" t="s">
@@ -21209,14 +21209,14 @@
       <c r="F118" s="13"/>
     </row>
     <row r="119" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A119" s="12" t="s">
+      <c r="A119" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B119" s="12"/>
-      <c r="C119" s="12"/>
-      <c r="D119" s="12"/>
-      <c r="E119" s="12"/>
-      <c r="F119" s="12"/>
+      <c r="B119" s="16"/>
+      <c r="C119" s="16"/>
+      <c r="D119" s="16"/>
+      <c r="E119" s="16"/>
+      <c r="F119" s="16"/>
     </row>
     <row r="120" spans="1:6" ht="34.5" customHeight="1">
       <c r="A120" s="13" t="s">
@@ -21229,14 +21229,14 @@
       <c r="F120" s="13"/>
     </row>
     <row r="121" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A121" s="12" t="s">
+      <c r="A121" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B121" s="12"/>
-      <c r="C121" s="12"/>
-      <c r="D121" s="12"/>
-      <c r="E121" s="12"/>
-      <c r="F121" s="12"/>
+      <c r="B121" s="16"/>
+      <c r="C121" s="16"/>
+      <c r="D121" s="16"/>
+      <c r="E121" s="16"/>
+      <c r="F121" s="16"/>
     </row>
     <row r="122" spans="1:6" ht="13.5" customHeight="1">
       <c r="A122" s="13" t="s">
@@ -21249,24 +21249,24 @@
       <c r="F122" s="13"/>
     </row>
     <row r="123" spans="1:6" ht="33" customHeight="1">
-      <c r="A123" s="12" t="s">
+      <c r="A123" s="16" t="s">
         <v>443</v>
       </c>
-      <c r="B123" s="12"/>
-      <c r="C123" s="12"/>
-      <c r="D123" s="12"/>
-      <c r="E123" s="12"/>
-      <c r="F123" s="12"/>
+      <c r="B123" s="16"/>
+      <c r="C123" s="16"/>
+      <c r="D123" s="16"/>
+      <c r="E123" s="16"/>
+      <c r="F123" s="16"/>
     </row>
     <row r="124" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A124" s="12" t="s">
+      <c r="A124" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B124" s="12"/>
-      <c r="C124" s="12"/>
-      <c r="D124" s="12"/>
-      <c r="E124" s="12"/>
-      <c r="F124" s="12"/>
+      <c r="B124" s="16"/>
+      <c r="C124" s="16"/>
+      <c r="D124" s="16"/>
+      <c r="E124" s="16"/>
+      <c r="F124" s="16"/>
     </row>
     <row r="125" spans="1:6" ht="34.5" customHeight="1">
       <c r="A125" s="13" t="s">
@@ -21279,14 +21279,14 @@
       <c r="F125" s="13"/>
     </row>
     <row r="126" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A126" s="12" t="s">
+      <c r="A126" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B126" s="12"/>
-      <c r="C126" s="12"/>
-      <c r="D126" s="12"/>
-      <c r="E126" s="12"/>
-      <c r="F126" s="12"/>
+      <c r="B126" s="16"/>
+      <c r="C126" s="16"/>
+      <c r="D126" s="16"/>
+      <c r="E126" s="16"/>
+      <c r="F126" s="16"/>
     </row>
     <row r="127" spans="1:6" ht="34.5" customHeight="1">
       <c r="A127" s="13" t="s">
@@ -21299,14 +21299,14 @@
       <c r="F127" s="13"/>
     </row>
     <row r="128" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A128" s="12" t="s">
+      <c r="A128" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B128" s="12"/>
-      <c r="C128" s="12"/>
-      <c r="D128" s="12"/>
-      <c r="E128" s="12"/>
-      <c r="F128" s="12"/>
+      <c r="B128" s="16"/>
+      <c r="C128" s="16"/>
+      <c r="D128" s="16"/>
+      <c r="E128" s="16"/>
+      <c r="F128" s="16"/>
     </row>
     <row r="129" spans="1:6" ht="34.5" customHeight="1">
       <c r="A129" s="13" t="s">
@@ -21319,14 +21319,14 @@
       <c r="F129" s="13"/>
     </row>
     <row r="130" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A130" s="12" t="s">
+      <c r="A130" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B130" s="12"/>
-      <c r="C130" s="12"/>
-      <c r="D130" s="12"/>
-      <c r="E130" s="12"/>
-      <c r="F130" s="12"/>
+      <c r="B130" s="16"/>
+      <c r="C130" s="16"/>
+      <c r="D130" s="16"/>
+      <c r="E130" s="16"/>
+      <c r="F130" s="16"/>
     </row>
     <row r="131" spans="1:6" ht="34.5" customHeight="1">
       <c r="A131" s="13" t="s">
@@ -21339,14 +21339,14 @@
       <c r="F131" s="13"/>
     </row>
     <row r="132" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A132" s="12" t="s">
+      <c r="A132" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B132" s="12"/>
-      <c r="C132" s="12"/>
-      <c r="D132" s="12"/>
-      <c r="E132" s="12"/>
-      <c r="F132" s="12"/>
+      <c r="B132" s="16"/>
+      <c r="C132" s="16"/>
+      <c r="D132" s="16"/>
+      <c r="E132" s="16"/>
+      <c r="F132" s="16"/>
     </row>
     <row r="133" spans="1:6" ht="34.5" customHeight="1">
       <c r="A133" s="13" t="s">
@@ -21369,14 +21369,14 @@
       <c r="F134" s="13"/>
     </row>
     <row r="135" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A135" s="12" t="s">
+      <c r="A135" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B135" s="12"/>
-      <c r="C135" s="12"/>
-      <c r="D135" s="12"/>
-      <c r="E135" s="12"/>
-      <c r="F135" s="12"/>
+      <c r="B135" s="16"/>
+      <c r="C135" s="16"/>
+      <c r="D135" s="16"/>
+      <c r="E135" s="16"/>
+      <c r="F135" s="16"/>
     </row>
     <row r="136" spans="1:6" ht="34.5" customHeight="1">
       <c r="A136" s="13" t="s">
@@ -21389,14 +21389,14 @@
       <c r="F136" s="13"/>
     </row>
     <row r="137" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A137" s="12" t="s">
+      <c r="A137" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B137" s="12"/>
-      <c r="C137" s="12"/>
-      <c r="D137" s="12"/>
-      <c r="E137" s="12"/>
-      <c r="F137" s="12"/>
+      <c r="B137" s="16"/>
+      <c r="C137" s="16"/>
+      <c r="D137" s="16"/>
+      <c r="E137" s="16"/>
+      <c r="F137" s="16"/>
     </row>
     <row r="138" spans="1:6" ht="34.5" customHeight="1">
       <c r="A138" s="13" t="s">
@@ -21409,14 +21409,14 @@
       <c r="F138" s="13"/>
     </row>
     <row r="139" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A139" s="12" t="s">
+      <c r="A139" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B139" s="12"/>
-      <c r="C139" s="12"/>
-      <c r="D139" s="12"/>
-      <c r="E139" s="12"/>
-      <c r="F139" s="12"/>
+      <c r="B139" s="16"/>
+      <c r="C139" s="16"/>
+      <c r="D139" s="16"/>
+      <c r="E139" s="16"/>
+      <c r="F139" s="16"/>
     </row>
     <row r="140" spans="1:6" ht="34.5" customHeight="1">
       <c r="A140" s="13" t="s">
@@ -21429,14 +21429,14 @@
       <c r="F140" s="13"/>
     </row>
     <row r="141" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A141" s="12" t="s">
+      <c r="A141" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B141" s="12"/>
-      <c r="C141" s="12"/>
-      <c r="D141" s="12"/>
-      <c r="E141" s="12"/>
-      <c r="F141" s="12"/>
+      <c r="B141" s="16"/>
+      <c r="C141" s="16"/>
+      <c r="D141" s="16"/>
+      <c r="E141" s="16"/>
+      <c r="F141" s="16"/>
     </row>
     <row r="142" spans="1:6" ht="34.5" customHeight="1">
       <c r="A142" s="13" t="s">
@@ -21449,14 +21449,14 @@
       <c r="F142" s="13"/>
     </row>
     <row r="143" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A143" s="12" t="s">
+      <c r="A143" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B143" s="12"/>
-      <c r="C143" s="12"/>
-      <c r="D143" s="12"/>
-      <c r="E143" s="12"/>
-      <c r="F143" s="12"/>
+      <c r="B143" s="16"/>
+      <c r="C143" s="16"/>
+      <c r="D143" s="16"/>
+      <c r="E143" s="16"/>
+      <c r="F143" s="16"/>
     </row>
     <row r="144" spans="1:6" ht="34.5" customHeight="1">
       <c r="A144" s="13" t="s">
@@ -21469,14 +21469,14 @@
       <c r="F144" s="13"/>
     </row>
     <row r="145" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A145" s="12" t="s">
+      <c r="A145" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B145" s="12"/>
-      <c r="C145" s="12"/>
-      <c r="D145" s="12"/>
-      <c r="E145" s="12"/>
-      <c r="F145" s="12"/>
+      <c r="B145" s="16"/>
+      <c r="C145" s="16"/>
+      <c r="D145" s="16"/>
+      <c r="E145" s="16"/>
+      <c r="F145" s="16"/>
     </row>
     <row r="146" spans="1:6" ht="34.5" customHeight="1">
       <c r="A146" s="13" t="s">
@@ -21489,14 +21489,14 @@
       <c r="F146" s="13"/>
     </row>
     <row r="147" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A147" s="12" t="s">
+      <c r="A147" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B147" s="12"/>
-      <c r="C147" s="12"/>
-      <c r="D147" s="12"/>
-      <c r="E147" s="12"/>
-      <c r="F147" s="12"/>
+      <c r="B147" s="16"/>
+      <c r="C147" s="16"/>
+      <c r="D147" s="16"/>
+      <c r="E147" s="16"/>
+      <c r="F147" s="16"/>
     </row>
     <row r="148" spans="1:6" ht="34.5" customHeight="1">
       <c r="A148" s="13" t="s">
@@ -21509,14 +21509,14 @@
       <c r="F148" s="13"/>
     </row>
     <row r="149" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A149" s="12" t="s">
+      <c r="A149" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B149" s="12"/>
-      <c r="C149" s="12"/>
-      <c r="D149" s="12"/>
-      <c r="E149" s="12"/>
-      <c r="F149" s="12"/>
+      <c r="B149" s="16"/>
+      <c r="C149" s="16"/>
+      <c r="D149" s="16"/>
+      <c r="E149" s="16"/>
+      <c r="F149" s="16"/>
     </row>
     <row r="150" spans="1:6" ht="34.5" customHeight="1">
       <c r="A150" s="13" t="s">
@@ -21529,14 +21529,14 @@
       <c r="F150" s="13"/>
     </row>
     <row r="151" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A151" s="12" t="s">
+      <c r="A151" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B151" s="12"/>
-      <c r="C151" s="12"/>
-      <c r="D151" s="12"/>
-      <c r="E151" s="12"/>
-      <c r="F151" s="12"/>
+      <c r="B151" s="16"/>
+      <c r="C151" s="16"/>
+      <c r="D151" s="16"/>
+      <c r="E151" s="16"/>
+      <c r="F151" s="16"/>
     </row>
     <row r="152" spans="1:6" ht="34.5" customHeight="1">
       <c r="A152" s="13" t="s">
@@ -21549,14 +21549,14 @@
       <c r="F152" s="13"/>
     </row>
     <row r="153" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A153" s="12" t="s">
+      <c r="A153" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B153" s="12"/>
-      <c r="C153" s="12"/>
-      <c r="D153" s="12"/>
-      <c r="E153" s="12"/>
-      <c r="F153" s="12"/>
+      <c r="B153" s="16"/>
+      <c r="C153" s="16"/>
+      <c r="D153" s="16"/>
+      <c r="E153" s="16"/>
+      <c r="F153" s="16"/>
     </row>
     <row r="154" spans="1:6" ht="13.5" customHeight="1">
       <c r="A154" s="13" t="s">
@@ -21579,14 +21579,14 @@
       <c r="F155" s="13"/>
     </row>
     <row r="156" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A156" s="12" t="s">
+      <c r="A156" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B156" s="12"/>
-      <c r="C156" s="12"/>
-      <c r="D156" s="12"/>
-      <c r="E156" s="12"/>
-      <c r="F156" s="12"/>
+      <c r="B156" s="16"/>
+      <c r="C156" s="16"/>
+      <c r="D156" s="16"/>
+      <c r="E156" s="16"/>
+      <c r="F156" s="16"/>
     </row>
     <row r="157" spans="1:6" ht="34.5" customHeight="1">
       <c r="A157" s="13" t="s">
@@ -21599,14 +21599,14 @@
       <c r="F157" s="13"/>
     </row>
     <row r="158" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A158" s="12" t="s">
+      <c r="A158" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B158" s="12"/>
-      <c r="C158" s="12"/>
-      <c r="D158" s="12"/>
-      <c r="E158" s="12"/>
-      <c r="F158" s="12"/>
+      <c r="B158" s="16"/>
+      <c r="C158" s="16"/>
+      <c r="D158" s="16"/>
+      <c r="E158" s="16"/>
+      <c r="F158" s="16"/>
     </row>
     <row r="159" spans="1:6" ht="34.5" customHeight="1">
       <c r="A159" s="13" t="s">
@@ -21619,14 +21619,14 @@
       <c r="F159" s="13"/>
     </row>
     <row r="160" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A160" s="12" t="s">
+      <c r="A160" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B160" s="12"/>
-      <c r="C160" s="12"/>
-      <c r="D160" s="12"/>
-      <c r="E160" s="12"/>
-      <c r="F160" s="12"/>
+      <c r="B160" s="16"/>
+      <c r="C160" s="16"/>
+      <c r="D160" s="16"/>
+      <c r="E160" s="16"/>
+      <c r="F160" s="16"/>
     </row>
     <row r="161" spans="1:6" ht="66" customHeight="1">
       <c r="A161" s="13" t="s">
@@ -21659,14 +21659,14 @@
       <c r="F163" s="13"/>
     </row>
     <row r="164" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A164" s="12" t="s">
+      <c r="A164" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B164" s="12"/>
-      <c r="C164" s="12"/>
-      <c r="D164" s="12"/>
-      <c r="E164" s="12"/>
-      <c r="F164" s="12"/>
+      <c r="B164" s="16"/>
+      <c r="C164" s="16"/>
+      <c r="D164" s="16"/>
+      <c r="E164" s="16"/>
+      <c r="F164" s="16"/>
     </row>
     <row r="165" spans="1:6" ht="151.5" customHeight="1">
       <c r="A165" s="13" t="s">
@@ -21679,14 +21679,14 @@
       <c r="F165" s="13"/>
     </row>
     <row r="166" spans="1:6" ht="151.5" customHeight="1">
-      <c r="A166" s="16" t="s">
+      <c r="A166" s="19" t="s">
         <v>467</v>
       </c>
-      <c r="B166" s="16"/>
-      <c r="C166" s="16"/>
-      <c r="D166" s="16"/>
-      <c r="E166" s="16"/>
-      <c r="F166" s="16"/>
+      <c r="B166" s="19"/>
+      <c r="C166" s="19"/>
+      <c r="D166" s="19"/>
+      <c r="E166" s="19"/>
+      <c r="F166" s="19"/>
     </row>
     <row r="167" spans="1:6" ht="55.5" customHeight="1">
       <c r="A167" s="13" t="s">
@@ -21719,14 +21719,14 @@
       <c r="F169" s="13"/>
     </row>
     <row r="170" spans="1:6" ht="96" customHeight="1">
-      <c r="A170" s="14" t="s">
+      <c r="A170" s="20" t="s">
         <v>471</v>
       </c>
-      <c r="B170" s="14"/>
-      <c r="C170" s="14"/>
-      <c r="D170" s="14"/>
-      <c r="E170" s="14"/>
-      <c r="F170" s="14"/>
+      <c r="B170" s="20"/>
+      <c r="C170" s="20"/>
+      <c r="D170" s="20"/>
+      <c r="E170" s="20"/>
+      <c r="F170" s="20"/>
     </row>
     <row r="171" spans="1:6" ht="97.5" customHeight="1">
       <c r="A171" s="13" t="s">
@@ -21779,14 +21779,14 @@
       <c r="F175" s="13"/>
     </row>
     <row r="176" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A176" s="12" t="s">
+      <c r="A176" s="16" t="s">
         <v>477</v>
       </c>
-      <c r="B176" s="12"/>
-      <c r="C176" s="12"/>
-      <c r="D176" s="12"/>
-      <c r="E176" s="12"/>
-      <c r="F176" s="12"/>
+      <c r="B176" s="16"/>
+      <c r="C176" s="16"/>
+      <c r="D176" s="16"/>
+      <c r="E176" s="16"/>
+      <c r="F176" s="16"/>
     </row>
     <row r="177" spans="1:6" ht="34.5" customHeight="1">
       <c r="A177" s="13" t="s">
@@ -21799,14 +21799,14 @@
       <c r="F177" s="13"/>
     </row>
     <row r="178" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A178" s="12" t="s">
+      <c r="A178" s="16" t="s">
         <v>477</v>
       </c>
-      <c r="B178" s="12"/>
-      <c r="C178" s="12"/>
-      <c r="D178" s="12"/>
-      <c r="E178" s="12"/>
-      <c r="F178" s="12"/>
+      <c r="B178" s="16"/>
+      <c r="C178" s="16"/>
+      <c r="D178" s="16"/>
+      <c r="E178" s="16"/>
+      <c r="F178" s="16"/>
     </row>
     <row r="179" spans="1:6" ht="34.5" customHeight="1">
       <c r="A179" s="13" t="s">
@@ -21819,14 +21819,14 @@
       <c r="F179" s="13"/>
     </row>
     <row r="180" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A180" s="12" t="s">
+      <c r="A180" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B180" s="12"/>
-      <c r="C180" s="12"/>
-      <c r="D180" s="12"/>
-      <c r="E180" s="12"/>
-      <c r="F180" s="12"/>
+      <c r="B180" s="16"/>
+      <c r="C180" s="16"/>
+      <c r="D180" s="16"/>
+      <c r="E180" s="16"/>
+      <c r="F180" s="16"/>
     </row>
     <row r="181" spans="1:6" ht="139.5" customHeight="1">
       <c r="A181" s="13" t="s">
@@ -21889,14 +21889,14 @@
       <c r="F186" s="13"/>
     </row>
     <row r="187" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A187" s="12" t="s">
+      <c r="A187" s="16" t="s">
         <v>486</v>
       </c>
-      <c r="B187" s="12"/>
-      <c r="C187" s="12"/>
-      <c r="D187" s="12"/>
-      <c r="E187" s="12"/>
-      <c r="F187" s="12"/>
+      <c r="B187" s="16"/>
+      <c r="C187" s="16"/>
+      <c r="D187" s="16"/>
+      <c r="E187" s="16"/>
+      <c r="F187" s="16"/>
     </row>
     <row r="188" spans="1:6" ht="66" customHeight="1">
       <c r="A188" s="13" t="s">
@@ -21919,14 +21919,14 @@
       <c r="F189" s="13"/>
     </row>
     <row r="190" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A190" s="12" t="s">
+      <c r="A190" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B190" s="12"/>
-      <c r="C190" s="12"/>
-      <c r="D190" s="12"/>
-      <c r="E190" s="12"/>
-      <c r="F190" s="12"/>
+      <c r="B190" s="16"/>
+      <c r="C190" s="16"/>
+      <c r="D190" s="16"/>
+      <c r="E190" s="16"/>
+      <c r="F190" s="16"/>
     </row>
     <row r="191" spans="1:6" ht="34.5" customHeight="1">
       <c r="A191" s="13" t="s">
@@ -21939,14 +21939,14 @@
       <c r="F191" s="13"/>
     </row>
     <row r="192" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A192" s="12" t="s">
+      <c r="A192" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B192" s="12"/>
-      <c r="C192" s="12"/>
-      <c r="D192" s="12"/>
-      <c r="E192" s="12"/>
-      <c r="F192" s="12"/>
+      <c r="B192" s="16"/>
+      <c r="C192" s="16"/>
+      <c r="D192" s="16"/>
+      <c r="E192" s="16"/>
+      <c r="F192" s="16"/>
     </row>
     <row r="193" spans="1:6" ht="34.5" customHeight="1">
       <c r="A193" s="13" t="s">
@@ -21959,14 +21959,14 @@
       <c r="F193" s="13"/>
     </row>
     <row r="194" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A194" s="12" t="s">
+      <c r="A194" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B194" s="12"/>
-      <c r="C194" s="12"/>
-      <c r="D194" s="12"/>
-      <c r="E194" s="12"/>
-      <c r="F194" s="12"/>
+      <c r="B194" s="16"/>
+      <c r="C194" s="16"/>
+      <c r="D194" s="16"/>
+      <c r="E194" s="16"/>
+      <c r="F194" s="16"/>
     </row>
     <row r="195" spans="1:6" ht="34.5" customHeight="1">
       <c r="A195" s="13" t="s">
@@ -21979,14 +21979,14 @@
       <c r="F195" s="13"/>
     </row>
     <row r="196" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A196" s="12" t="s">
+      <c r="A196" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B196" s="12"/>
-      <c r="C196" s="12"/>
-      <c r="D196" s="12"/>
-      <c r="E196" s="12"/>
-      <c r="F196" s="12"/>
+      <c r="B196" s="16"/>
+      <c r="C196" s="16"/>
+      <c r="D196" s="16"/>
+      <c r="E196" s="16"/>
+      <c r="F196" s="16"/>
     </row>
     <row r="197" spans="1:6" ht="34.5" customHeight="1">
       <c r="A197" s="13" t="s">
@@ -21999,14 +21999,14 @@
       <c r="F197" s="13"/>
     </row>
     <row r="198" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A198" s="12" t="s">
+      <c r="A198" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B198" s="12"/>
-      <c r="C198" s="12"/>
-      <c r="D198" s="12"/>
-      <c r="E198" s="12"/>
-      <c r="F198" s="12"/>
+      <c r="B198" s="16"/>
+      <c r="C198" s="16"/>
+      <c r="D198" s="16"/>
+      <c r="E198" s="16"/>
+      <c r="F198" s="16"/>
     </row>
     <row r="199" spans="1:6" ht="66" customHeight="1">
       <c r="A199" s="13" t="s">
@@ -22029,14 +22029,14 @@
       <c r="F200" s="13"/>
     </row>
     <row r="201" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A201" s="12" t="s">
+      <c r="A201" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B201" s="12"/>
-      <c r="C201" s="12"/>
-      <c r="D201" s="12"/>
-      <c r="E201" s="12"/>
-      <c r="F201" s="12"/>
+      <c r="B201" s="16"/>
+      <c r="C201" s="16"/>
+      <c r="D201" s="16"/>
+      <c r="E201" s="16"/>
+      <c r="F201" s="16"/>
     </row>
     <row r="202" spans="1:6" ht="34.5" customHeight="1">
       <c r="A202" s="13" t="s">
@@ -22049,14 +22049,14 @@
       <c r="F202" s="13"/>
     </row>
     <row r="203" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A203" s="12" t="s">
+      <c r="A203" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B203" s="12"/>
-      <c r="C203" s="12"/>
-      <c r="D203" s="12"/>
-      <c r="E203" s="12"/>
-      <c r="F203" s="12"/>
+      <c r="B203" s="16"/>
+      <c r="C203" s="16"/>
+      <c r="D203" s="16"/>
+      <c r="E203" s="16"/>
+      <c r="F203" s="16"/>
     </row>
     <row r="204" spans="1:6" ht="97.5" customHeight="1">
       <c r="A204" s="13" t="s">
@@ -22079,14 +22079,14 @@
       <c r="F205" s="13"/>
     </row>
     <row r="206" spans="1:6" ht="54" customHeight="1">
-      <c r="A206" s="12" t="s">
+      <c r="A206" s="16" t="s">
         <v>498</v>
       </c>
-      <c r="B206" s="12"/>
-      <c r="C206" s="12"/>
-      <c r="D206" s="12"/>
-      <c r="E206" s="12"/>
-      <c r="F206" s="12"/>
+      <c r="B206" s="16"/>
+      <c r="C206" s="16"/>
+      <c r="D206" s="16"/>
+      <c r="E206" s="16"/>
+      <c r="F206" s="16"/>
     </row>
     <row r="207" spans="1:6" ht="66" customHeight="1">
       <c r="A207" s="13" t="s">
@@ -22109,14 +22109,14 @@
       <c r="F208" s="13"/>
     </row>
     <row r="209" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A209" s="12" t="s">
+      <c r="A209" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B209" s="12"/>
-      <c r="C209" s="12"/>
-      <c r="D209" s="12"/>
-      <c r="E209" s="12"/>
-      <c r="F209" s="12"/>
+      <c r="B209" s="16"/>
+      <c r="C209" s="16"/>
+      <c r="D209" s="16"/>
+      <c r="E209" s="16"/>
+      <c r="F209" s="16"/>
     </row>
     <row r="210" spans="1:6" ht="34.5" customHeight="1">
       <c r="A210" s="13" t="s">
@@ -22129,14 +22129,14 @@
       <c r="F210" s="13"/>
     </row>
     <row r="211" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A211" s="12" t="s">
+      <c r="A211" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B211" s="12"/>
-      <c r="C211" s="12"/>
-      <c r="D211" s="12"/>
-      <c r="E211" s="12"/>
-      <c r="F211" s="12"/>
+      <c r="B211" s="16"/>
+      <c r="C211" s="16"/>
+      <c r="D211" s="16"/>
+      <c r="E211" s="16"/>
+      <c r="F211" s="16"/>
     </row>
     <row r="212" spans="1:6" ht="66" customHeight="1">
       <c r="A212" s="13" t="s">
@@ -22159,14 +22159,14 @@
       <c r="F213" s="13"/>
     </row>
     <row r="214" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A214" s="12" t="s">
+      <c r="A214" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B214" s="12"/>
-      <c r="C214" s="12"/>
-      <c r="D214" s="12"/>
-      <c r="E214" s="12"/>
-      <c r="F214" s="12"/>
+      <c r="B214" s="16"/>
+      <c r="C214" s="16"/>
+      <c r="D214" s="16"/>
+      <c r="E214" s="16"/>
+      <c r="F214" s="16"/>
     </row>
     <row r="215" spans="1:6" ht="34.5" customHeight="1">
       <c r="A215" s="13" t="s">
@@ -22179,14 +22179,14 @@
       <c r="F215" s="13"/>
     </row>
     <row r="216" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A216" s="12" t="s">
+      <c r="A216" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B216" s="12"/>
-      <c r="C216" s="12"/>
-      <c r="D216" s="12"/>
-      <c r="E216" s="12"/>
-      <c r="F216" s="12"/>
+      <c r="B216" s="16"/>
+      <c r="C216" s="16"/>
+      <c r="D216" s="16"/>
+      <c r="E216" s="16"/>
+      <c r="F216" s="16"/>
     </row>
     <row r="217" spans="1:6" ht="34.5" customHeight="1">
       <c r="A217" s="13" t="s">
@@ -22199,14 +22199,14 @@
       <c r="F217" s="13"/>
     </row>
     <row r="218" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A218" s="12" t="s">
+      <c r="A218" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B218" s="12"/>
-      <c r="C218" s="12"/>
-      <c r="D218" s="12"/>
-      <c r="E218" s="12"/>
-      <c r="F218" s="12"/>
+      <c r="B218" s="16"/>
+      <c r="C218" s="16"/>
+      <c r="D218" s="16"/>
+      <c r="E218" s="16"/>
+      <c r="F218" s="16"/>
     </row>
     <row r="219" spans="1:6" ht="34.5" customHeight="1">
       <c r="A219" s="13" t="s">
@@ -22219,14 +22219,14 @@
       <c r="F219" s="13"/>
     </row>
     <row r="220" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A220" s="12" t="s">
+      <c r="A220" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="B220" s="12"/>
-      <c r="C220" s="12"/>
-      <c r="D220" s="12"/>
-      <c r="E220" s="12"/>
-      <c r="F220" s="12"/>
+      <c r="B220" s="16"/>
+      <c r="C220" s="16"/>
+      <c r="D220" s="16"/>
+      <c r="E220" s="16"/>
+      <c r="F220" s="16"/>
     </row>
     <row r="221" spans="1:6" ht="34.5" customHeight="1">
       <c r="A221" s="13" t="s">
@@ -22239,14 +22239,14 @@
       <c r="F221" s="13"/>
     </row>
     <row r="222" spans="1:6" ht="33" customHeight="1">
-      <c r="A222" s="12" t="s">
+      <c r="A222" s="16" t="s">
         <v>508</v>
       </c>
-      <c r="B222" s="12"/>
-      <c r="C222" s="12"/>
-      <c r="D222" s="12"/>
-      <c r="E222" s="12"/>
-      <c r="F222" s="12"/>
+      <c r="B222" s="16"/>
+      <c r="C222" s="16"/>
+      <c r="D222" s="16"/>
+      <c r="E222" s="16"/>
+      <c r="F222" s="16"/>
     </row>
     <row r="223" spans="1:6" ht="34.5" customHeight="1">
       <c r="A223" s="13" t="s">
@@ -22259,14 +22259,14 @@
       <c r="F223" s="13"/>
     </row>
     <row r="224" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A224" s="12" t="s">
+      <c r="A224" s="16" t="s">
         <v>510</v>
       </c>
-      <c r="B224" s="12"/>
-      <c r="C224" s="12"/>
-      <c r="D224" s="12"/>
-      <c r="E224" s="12"/>
-      <c r="F224" s="12"/>
+      <c r="B224" s="16"/>
+      <c r="C224" s="16"/>
+      <c r="D224" s="16"/>
+      <c r="E224" s="16"/>
+      <c r="F224" s="16"/>
     </row>
     <row r="225" spans="1:6" ht="34.5" customHeight="1">
       <c r="A225" s="13" t="s">
@@ -22359,14 +22359,14 @@
       <c r="F233" s="13"/>
     </row>
     <row r="234" spans="1:6" ht="33" customHeight="1">
-      <c r="A234" s="12" t="s">
+      <c r="A234" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="B234" s="12"/>
-      <c r="C234" s="12"/>
-      <c r="D234" s="12"/>
-      <c r="E234" s="12"/>
-      <c r="F234" s="12"/>
+      <c r="B234" s="16"/>
+      <c r="C234" s="16"/>
+      <c r="D234" s="16"/>
+      <c r="E234" s="16"/>
+      <c r="F234" s="16"/>
     </row>
     <row r="235" spans="1:6" ht="55.5" customHeight="1">
       <c r="A235" s="13" t="s">
@@ -22479,14 +22479,14 @@
       <c r="F245" s="13"/>
     </row>
     <row r="246" spans="1:6" ht="33" customHeight="1">
-      <c r="A246" s="12" t="s">
+      <c r="A246" s="16" t="s">
         <v>531</v>
       </c>
-      <c r="B246" s="12"/>
-      <c r="C246" s="12"/>
-      <c r="D246" s="12"/>
-      <c r="E246" s="12"/>
-      <c r="F246" s="12"/>
+      <c r="B246" s="16"/>
+      <c r="C246" s="16"/>
+      <c r="D246" s="16"/>
+      <c r="E246" s="16"/>
+      <c r="F246" s="16"/>
     </row>
     <row r="247" spans="1:6" ht="34.5" customHeight="1">
       <c r="A247" s="13" t="s">
@@ -22499,14 +22499,14 @@
       <c r="F247" s="13"/>
     </row>
     <row r="248" spans="1:6" ht="33" customHeight="1">
-      <c r="A248" s="12" t="s">
+      <c r="A248" s="16" t="s">
         <v>533</v>
       </c>
-      <c r="B248" s="12"/>
-      <c r="C248" s="12"/>
-      <c r="D248" s="12"/>
-      <c r="E248" s="12"/>
-      <c r="F248" s="12"/>
+      <c r="B248" s="16"/>
+      <c r="C248" s="16"/>
+      <c r="D248" s="16"/>
+      <c r="E248" s="16"/>
+      <c r="F248" s="16"/>
     </row>
     <row r="249" spans="1:6" ht="34.5" customHeight="1">
       <c r="A249" s="13" t="s">
@@ -22519,14 +22519,14 @@
       <c r="F249" s="13"/>
     </row>
     <row r="250" spans="1:6" ht="33" customHeight="1">
-      <c r="A250" s="12" t="s">
+      <c r="A250" s="16" t="s">
         <v>535</v>
       </c>
-      <c r="B250" s="12"/>
-      <c r="C250" s="12"/>
-      <c r="D250" s="12"/>
-      <c r="E250" s="12"/>
-      <c r="F250" s="12"/>
+      <c r="B250" s="16"/>
+      <c r="C250" s="16"/>
+      <c r="D250" s="16"/>
+      <c r="E250" s="16"/>
+      <c r="F250" s="16"/>
     </row>
     <row r="251" spans="1:6" ht="34.5" customHeight="1">
       <c r="A251" s="13" t="s">
@@ -22539,14 +22539,14 @@
       <c r="F251" s="13"/>
     </row>
     <row r="252" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A252" s="12" t="s">
+      <c r="A252" s="16" t="s">
         <v>537</v>
       </c>
-      <c r="B252" s="12"/>
-      <c r="C252" s="12"/>
-      <c r="D252" s="12"/>
-      <c r="E252" s="12"/>
-      <c r="F252" s="12"/>
+      <c r="B252" s="16"/>
+      <c r="C252" s="16"/>
+      <c r="D252" s="16"/>
+      <c r="E252" s="16"/>
+      <c r="F252" s="16"/>
     </row>
     <row r="253" spans="1:6" ht="66" customHeight="1">
       <c r="A253" s="13" t="s">
@@ -22629,14 +22629,14 @@
       <c r="F260" s="13"/>
     </row>
     <row r="261" spans="1:6" ht="33" customHeight="1">
-      <c r="A261" s="12" t="s">
+      <c r="A261" s="16" t="s">
         <v>546</v>
       </c>
-      <c r="B261" s="12"/>
-      <c r="C261" s="12"/>
-      <c r="D261" s="12"/>
-      <c r="E261" s="12"/>
-      <c r="F261" s="12"/>
+      <c r="B261" s="16"/>
+      <c r="C261" s="16"/>
+      <c r="D261" s="16"/>
+      <c r="E261" s="16"/>
+      <c r="F261" s="16"/>
     </row>
     <row r="262" spans="1:6" ht="34.5" customHeight="1">
       <c r="A262" s="13" t="s">
@@ -22649,14 +22649,14 @@
       <c r="F262" s="13"/>
     </row>
     <row r="263" spans="1:6" ht="33" customHeight="1">
-      <c r="A263" s="12" t="s">
+      <c r="A263" s="16" t="s">
         <v>548</v>
       </c>
-      <c r="B263" s="12"/>
-      <c r="C263" s="12"/>
-      <c r="D263" s="12"/>
-      <c r="E263" s="12"/>
-      <c r="F263" s="12"/>
+      <c r="B263" s="16"/>
+      <c r="C263" s="16"/>
+      <c r="D263" s="16"/>
+      <c r="E263" s="16"/>
+      <c r="F263" s="16"/>
     </row>
     <row r="264" spans="1:6" ht="66" customHeight="1">
       <c r="A264" s="13" t="s">
@@ -22679,14 +22679,14 @@
       <c r="F265" s="13"/>
     </row>
     <row r="266" spans="1:6" ht="33" customHeight="1">
-      <c r="A266" s="12" t="s">
+      <c r="A266" s="16" t="s">
         <v>551</v>
       </c>
-      <c r="B266" s="12"/>
-      <c r="C266" s="12"/>
-      <c r="D266" s="12"/>
-      <c r="E266" s="12"/>
-      <c r="F266" s="12"/>
+      <c r="B266" s="16"/>
+      <c r="C266" s="16"/>
+      <c r="D266" s="16"/>
+      <c r="E266" s="16"/>
+      <c r="F266" s="16"/>
     </row>
     <row r="267" spans="1:6" ht="34.5" customHeight="1">
       <c r="A267" s="13" t="s">
@@ -22699,14 +22699,14 @@
       <c r="F267" s="13"/>
     </row>
     <row r="268" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A268" s="12" t="s">
+      <c r="A268" s="16" t="s">
         <v>553</v>
       </c>
-      <c r="B268" s="12"/>
-      <c r="C268" s="12"/>
-      <c r="D268" s="12"/>
-      <c r="E268" s="12"/>
-      <c r="F268" s="12"/>
+      <c r="B268" s="16"/>
+      <c r="C268" s="16"/>
+      <c r="D268" s="16"/>
+      <c r="E268" s="16"/>
+      <c r="F268" s="16"/>
     </row>
     <row r="269" spans="1:6" ht="118.5" customHeight="1">
       <c r="A269" s="13" t="s">
@@ -22729,14 +22729,14 @@
       <c r="F270" s="13"/>
     </row>
     <row r="271" spans="1:6" ht="96" customHeight="1">
-      <c r="A271" s="12" t="s">
+      <c r="A271" s="16" t="s">
         <v>556</v>
       </c>
-      <c r="B271" s="12"/>
-      <c r="C271" s="12"/>
-      <c r="D271" s="12"/>
-      <c r="E271" s="12"/>
-      <c r="F271" s="12"/>
+      <c r="B271" s="16"/>
+      <c r="C271" s="16"/>
+      <c r="D271" s="16"/>
+      <c r="E271" s="16"/>
+      <c r="F271" s="16"/>
     </row>
     <row r="272" spans="1:6" ht="34.5" customHeight="1">
       <c r="A272" s="13" t="s">
@@ -22749,24 +22749,24 @@
       <c r="F272" s="13"/>
     </row>
     <row r="273" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A273" s="12" t="s">
+      <c r="A273" s="16" t="s">
         <v>558</v>
       </c>
-      <c r="B273" s="12"/>
-      <c r="C273" s="12"/>
-      <c r="D273" s="12"/>
-      <c r="E273" s="12"/>
-      <c r="F273" s="12"/>
+      <c r="B273" s="16"/>
+      <c r="C273" s="16"/>
+      <c r="D273" s="16"/>
+      <c r="E273" s="16"/>
+      <c r="F273" s="16"/>
     </row>
     <row r="274" spans="1:6" ht="85.5" customHeight="1">
-      <c r="A274" s="12" t="s">
+      <c r="A274" s="16" t="s">
         <v>559</v>
       </c>
-      <c r="B274" s="12"/>
-      <c r="C274" s="12"/>
-      <c r="D274" s="12"/>
-      <c r="E274" s="12"/>
-      <c r="F274" s="12"/>
+      <c r="B274" s="16"/>
+      <c r="C274" s="16"/>
+      <c r="D274" s="16"/>
+      <c r="E274" s="16"/>
+      <c r="F274" s="16"/>
     </row>
     <row r="275" spans="1:6" ht="34.5" customHeight="1">
       <c r="A275" s="13" t="s">
@@ -22779,14 +22779,14 @@
       <c r="F275" s="13"/>
     </row>
     <row r="276" spans="1:6" ht="96" customHeight="1">
-      <c r="A276" s="12" t="s">
+      <c r="A276" s="16" t="s">
         <v>556</v>
       </c>
-      <c r="B276" s="12"/>
-      <c r="C276" s="12"/>
-      <c r="D276" s="12"/>
-      <c r="E276" s="12"/>
-      <c r="F276" s="12"/>
+      <c r="B276" s="16"/>
+      <c r="C276" s="16"/>
+      <c r="D276" s="16"/>
+      <c r="E276" s="16"/>
+      <c r="F276" s="16"/>
     </row>
     <row r="277" spans="1:6" ht="118.5" customHeight="1">
       <c r="A277" s="13" t="s">
@@ -22809,24 +22809,24 @@
       <c r="F278" s="13"/>
     </row>
     <row r="279" spans="1:6" ht="33" customHeight="1">
-      <c r="A279" s="12" t="s">
+      <c r="A279" s="16" t="s">
         <v>563</v>
       </c>
-      <c r="B279" s="12"/>
-      <c r="C279" s="12"/>
-      <c r="D279" s="12"/>
-      <c r="E279" s="12"/>
-      <c r="F279" s="12"/>
+      <c r="B279" s="16"/>
+      <c r="C279" s="16"/>
+      <c r="D279" s="16"/>
+      <c r="E279" s="16"/>
+      <c r="F279" s="16"/>
     </row>
     <row r="280" spans="1:6" ht="75" customHeight="1">
-      <c r="A280" s="14" t="s">
+      <c r="A280" s="20" t="s">
         <v>564</v>
       </c>
-      <c r="B280" s="14"/>
-      <c r="C280" s="14"/>
-      <c r="D280" s="14"/>
-      <c r="E280" s="14"/>
-      <c r="F280" s="14"/>
+      <c r="B280" s="20"/>
+      <c r="C280" s="20"/>
+      <c r="D280" s="20"/>
+      <c r="E280" s="20"/>
+      <c r="F280" s="20"/>
     </row>
     <row r="281" spans="1:6" ht="34.5" customHeight="1">
       <c r="A281" s="13" t="s">
@@ -22839,14 +22839,14 @@
       <c r="F281" s="13"/>
     </row>
     <row r="282" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A282" s="12" t="s">
+      <c r="A282" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="B282" s="12"/>
-      <c r="C282" s="12"/>
-      <c r="D282" s="12"/>
-      <c r="E282" s="12"/>
-      <c r="F282" s="12"/>
+      <c r="B282" s="16"/>
+      <c r="C282" s="16"/>
+      <c r="D282" s="16"/>
+      <c r="E282" s="16"/>
+      <c r="F282" s="16"/>
     </row>
     <row r="283" spans="1:6" ht="34.5" customHeight="1">
       <c r="A283" s="13" t="s">
@@ -22859,14 +22859,14 @@
       <c r="F283" s="13"/>
     </row>
     <row r="284" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A284" s="12" t="s">
+      <c r="A284" s="16" t="s">
         <v>568</v>
       </c>
-      <c r="B284" s="12"/>
-      <c r="C284" s="12"/>
-      <c r="D284" s="12"/>
-      <c r="E284" s="12"/>
-      <c r="F284" s="12"/>
+      <c r="B284" s="16"/>
+      <c r="C284" s="16"/>
+      <c r="D284" s="16"/>
+      <c r="E284" s="16"/>
+      <c r="F284" s="16"/>
     </row>
     <row r="285" spans="1:6" ht="45" customHeight="1">
       <c r="A285" s="13" t="s">
@@ -22879,14 +22879,14 @@
       <c r="F285" s="13"/>
     </row>
     <row r="286" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A286" s="12" t="s">
+      <c r="A286" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="B286" s="12"/>
-      <c r="C286" s="12"/>
-      <c r="D286" s="12"/>
-      <c r="E286" s="12"/>
-      <c r="F286" s="12"/>
+      <c r="B286" s="16"/>
+      <c r="C286" s="16"/>
+      <c r="D286" s="16"/>
+      <c r="E286" s="16"/>
+      <c r="F286" s="16"/>
     </row>
     <row r="287" spans="1:6" ht="45" customHeight="1">
       <c r="A287" s="13" t="s">
@@ -22899,14 +22899,14 @@
       <c r="F287" s="13"/>
     </row>
     <row r="288" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A288" s="12" t="s">
+      <c r="A288" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="B288" s="12"/>
-      <c r="C288" s="12"/>
-      <c r="D288" s="12"/>
-      <c r="E288" s="12"/>
-      <c r="F288" s="12"/>
+      <c r="B288" s="16"/>
+      <c r="C288" s="16"/>
+      <c r="D288" s="16"/>
+      <c r="E288" s="16"/>
+      <c r="F288" s="16"/>
     </row>
     <row r="289" spans="1:6" ht="13.5" customHeight="1">
       <c r="A289" s="13" t="s">
@@ -22919,24 +22919,24 @@
       <c r="F289" s="13"/>
     </row>
     <row r="290" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A290" s="12" t="s">
+      <c r="A290" s="16" t="s">
         <v>574</v>
       </c>
-      <c r="B290" s="12"/>
-      <c r="C290" s="12"/>
-      <c r="D290" s="12"/>
-      <c r="E290" s="12"/>
-      <c r="F290" s="12"/>
+      <c r="B290" s="16"/>
+      <c r="C290" s="16"/>
+      <c r="D290" s="16"/>
+      <c r="E290" s="16"/>
+      <c r="F290" s="16"/>
     </row>
     <row r="291" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A291" s="12" t="s">
+      <c r="A291" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="B291" s="12"/>
-      <c r="C291" s="12"/>
-      <c r="D291" s="12"/>
-      <c r="E291" s="12"/>
-      <c r="F291" s="12"/>
+      <c r="B291" s="16"/>
+      <c r="C291" s="16"/>
+      <c r="D291" s="16"/>
+      <c r="E291" s="16"/>
+      <c r="F291" s="16"/>
     </row>
     <row r="292" spans="1:6" ht="34.5" customHeight="1">
       <c r="A292" s="13" t="s">
@@ -22949,14 +22949,14 @@
       <c r="F292" s="13"/>
     </row>
     <row r="293" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A293" s="12" t="s">
+      <c r="A293" s="16" t="s">
         <v>576</v>
       </c>
-      <c r="B293" s="12"/>
-      <c r="C293" s="12"/>
-      <c r="D293" s="12"/>
-      <c r="E293" s="12"/>
-      <c r="F293" s="12"/>
+      <c r="B293" s="16"/>
+      <c r="C293" s="16"/>
+      <c r="D293" s="16"/>
+      <c r="E293" s="16"/>
+      <c r="F293" s="16"/>
     </row>
     <row r="294" spans="1:6" ht="45" customHeight="1">
       <c r="A294" s="13" t="s">
@@ -22969,14 +22969,14 @@
       <c r="F294" s="13"/>
     </row>
     <row r="295" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A295" s="12" t="s">
+      <c r="A295" s="16" t="s">
         <v>576</v>
       </c>
-      <c r="B295" s="12"/>
-      <c r="C295" s="12"/>
-      <c r="D295" s="12"/>
-      <c r="E295" s="12"/>
-      <c r="F295" s="12"/>
+      <c r="B295" s="16"/>
+      <c r="C295" s="16"/>
+      <c r="D295" s="16"/>
+      <c r="E295" s="16"/>
+      <c r="F295" s="16"/>
     </row>
     <row r="296" spans="1:6" ht="34.5" customHeight="1">
       <c r="A296" s="13" t="s">
@@ -22989,14 +22989,14 @@
       <c r="F296" s="13"/>
     </row>
     <row r="297" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A297" s="12" t="s">
+      <c r="A297" s="16" t="s">
         <v>579</v>
       </c>
-      <c r="B297" s="12"/>
-      <c r="C297" s="12"/>
-      <c r="D297" s="12"/>
-      <c r="E297" s="12"/>
-      <c r="F297" s="12"/>
+      <c r="B297" s="16"/>
+      <c r="C297" s="16"/>
+      <c r="D297" s="16"/>
+      <c r="E297" s="16"/>
+      <c r="F297" s="16"/>
     </row>
     <row r="298" spans="1:6" ht="34.5" customHeight="1">
       <c r="A298" s="13" t="s">
@@ -23009,14 +23009,14 @@
       <c r="F298" s="13"/>
     </row>
     <row r="299" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A299" s="12" t="s">
+      <c r="A299" s="16" t="s">
         <v>581</v>
       </c>
-      <c r="B299" s="12"/>
-      <c r="C299" s="12"/>
-      <c r="D299" s="12"/>
-      <c r="E299" s="12"/>
-      <c r="F299" s="12"/>
+      <c r="B299" s="16"/>
+      <c r="C299" s="16"/>
+      <c r="D299" s="16"/>
+      <c r="E299" s="16"/>
+      <c r="F299" s="16"/>
     </row>
     <row r="300" spans="1:6" ht="45" customHeight="1">
       <c r="A300" s="13" t="s">
@@ -23029,14 +23029,14 @@
       <c r="F300" s="13"/>
     </row>
     <row r="301" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A301" s="12" t="s">
+      <c r="A301" s="16" t="s">
         <v>583</v>
       </c>
-      <c r="B301" s="12"/>
-      <c r="C301" s="12"/>
-      <c r="D301" s="12"/>
-      <c r="E301" s="12"/>
-      <c r="F301" s="12"/>
+      <c r="B301" s="16"/>
+      <c r="C301" s="16"/>
+      <c r="D301" s="16"/>
+      <c r="E301" s="16"/>
+      <c r="F301" s="16"/>
     </row>
     <row r="302" spans="1:6" ht="45" customHeight="1">
       <c r="A302" s="13" t="s">
@@ -23049,14 +23049,14 @@
       <c r="F302" s="13"/>
     </row>
     <row r="303" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A303" s="12" t="s">
+      <c r="A303" s="16" t="s">
         <v>585</v>
       </c>
-      <c r="B303" s="12"/>
-      <c r="C303" s="12"/>
-      <c r="D303" s="12"/>
-      <c r="E303" s="12"/>
-      <c r="F303" s="12"/>
+      <c r="B303" s="16"/>
+      <c r="C303" s="16"/>
+      <c r="D303" s="16"/>
+      <c r="E303" s="16"/>
+      <c r="F303" s="16"/>
     </row>
     <row r="304" spans="1:6" ht="55.5" customHeight="1">
       <c r="A304" s="13" t="s">
@@ -23069,14 +23069,14 @@
       <c r="F304" s="13"/>
     </row>
     <row r="305" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A305" s="12" t="s">
+      <c r="A305" s="16" t="s">
         <v>585</v>
       </c>
-      <c r="B305" s="12"/>
-      <c r="C305" s="12"/>
-      <c r="D305" s="12"/>
-      <c r="E305" s="12"/>
-      <c r="F305" s="12"/>
+      <c r="B305" s="16"/>
+      <c r="C305" s="16"/>
+      <c r="D305" s="16"/>
+      <c r="E305" s="16"/>
+      <c r="F305" s="16"/>
     </row>
     <row r="306" spans="1:6" ht="34.5" customHeight="1">
       <c r="A306" s="13" t="s">
@@ -23089,14 +23089,14 @@
       <c r="F306" s="13"/>
     </row>
     <row r="307" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A307" s="12" t="s">
+      <c r="A307" s="16" t="s">
         <v>585</v>
       </c>
-      <c r="B307" s="12"/>
-      <c r="C307" s="12"/>
-      <c r="D307" s="12"/>
-      <c r="E307" s="12"/>
-      <c r="F307" s="12"/>
+      <c r="B307" s="16"/>
+      <c r="C307" s="16"/>
+      <c r="D307" s="16"/>
+      <c r="E307" s="16"/>
+      <c r="F307" s="16"/>
     </row>
     <row r="308" spans="1:6" ht="45" customHeight="1">
       <c r="A308" s="13" t="s">
@@ -23109,14 +23109,14 @@
       <c r="F308" s="13"/>
     </row>
     <row r="309" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A309" s="12" t="s">
+      <c r="A309" s="16" t="s">
         <v>581</v>
       </c>
-      <c r="B309" s="12"/>
-      <c r="C309" s="12"/>
-      <c r="D309" s="12"/>
-      <c r="E309" s="12"/>
-      <c r="F309" s="12"/>
+      <c r="B309" s="16"/>
+      <c r="C309" s="16"/>
+      <c r="D309" s="16"/>
+      <c r="E309" s="16"/>
+      <c r="F309" s="16"/>
     </row>
     <row r="310" spans="1:6" ht="55.5" customHeight="1">
       <c r="A310" s="13" t="s">
@@ -23129,14 +23129,14 @@
       <c r="F310" s="13"/>
     </row>
     <row r="311" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A311" s="14" t="s">
+      <c r="A311" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="B311" s="14"/>
-      <c r="C311" s="14"/>
-      <c r="D311" s="14"/>
-      <c r="E311" s="14"/>
-      <c r="F311" s="14"/>
+      <c r="B311" s="20"/>
+      <c r="C311" s="20"/>
+      <c r="D311" s="20"/>
+      <c r="E311" s="20"/>
+      <c r="F311" s="20"/>
     </row>
     <row r="312" spans="1:6" ht="45" customHeight="1">
       <c r="A312" s="13" t="s">
@@ -23149,14 +23149,14 @@
       <c r="F312" s="13"/>
     </row>
     <row r="313" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A313" s="12" t="s">
+      <c r="A313" s="16" t="s">
         <v>553</v>
       </c>
-      <c r="B313" s="12"/>
-      <c r="C313" s="12"/>
-      <c r="D313" s="12"/>
-      <c r="E313" s="12"/>
-      <c r="F313" s="12"/>
+      <c r="B313" s="16"/>
+      <c r="C313" s="16"/>
+      <c r="D313" s="16"/>
+      <c r="E313" s="16"/>
+      <c r="F313" s="16"/>
     </row>
     <row r="314" spans="1:6" ht="76.5" customHeight="1">
       <c r="A314" s="15" t="s">
@@ -23199,14 +23199,14 @@
       <c r="F317" s="13"/>
     </row>
     <row r="318" spans="1:6" ht="96" customHeight="1">
-      <c r="A318" s="12" t="s">
+      <c r="A318" s="16" t="s">
         <v>596</v>
       </c>
-      <c r="B318" s="12"/>
-      <c r="C318" s="12"/>
-      <c r="D318" s="12"/>
-      <c r="E318" s="12"/>
-      <c r="F318" s="12"/>
+      <c r="B318" s="16"/>
+      <c r="C318" s="16"/>
+      <c r="D318" s="16"/>
+      <c r="E318" s="16"/>
+      <c r="F318" s="16"/>
     </row>
     <row r="319" spans="1:6" ht="55.5" customHeight="1">
       <c r="A319" s="13" t="s">
@@ -23229,14 +23229,14 @@
       <c r="F320" s="13"/>
     </row>
     <row r="321" spans="1:6" ht="33" customHeight="1">
-      <c r="A321" s="12" t="s">
+      <c r="A321" s="16" t="s">
         <v>599</v>
       </c>
-      <c r="B321" s="12"/>
-      <c r="C321" s="12"/>
-      <c r="D321" s="12"/>
-      <c r="E321" s="12"/>
-      <c r="F321" s="12"/>
+      <c r="B321" s="16"/>
+      <c r="C321" s="16"/>
+      <c r="D321" s="16"/>
+      <c r="E321" s="16"/>
+      <c r="F321" s="16"/>
     </row>
     <row r="322" spans="1:6" ht="45" customHeight="1">
       <c r="A322" s="13" t="s">
@@ -23299,14 +23299,14 @@
       <c r="F327" s="13"/>
     </row>
     <row r="328" spans="1:6" ht="75" customHeight="1">
-      <c r="A328" s="12" t="s">
+      <c r="A328" s="16" t="s">
         <v>606</v>
       </c>
-      <c r="B328" s="12"/>
-      <c r="C328" s="12"/>
-      <c r="D328" s="12"/>
-      <c r="E328" s="12"/>
-      <c r="F328" s="12"/>
+      <c r="B328" s="16"/>
+      <c r="C328" s="16"/>
+      <c r="D328" s="16"/>
+      <c r="E328" s="16"/>
+      <c r="F328" s="16"/>
     </row>
     <row r="329" spans="1:6" ht="97.5" customHeight="1">
       <c r="A329" s="13" t="s">
@@ -23339,14 +23339,14 @@
       <c r="F331" s="13"/>
     </row>
     <row r="332" spans="1:6" ht="85.5" customHeight="1">
-      <c r="A332" s="12" t="s">
+      <c r="A332" s="16" t="s">
         <v>610</v>
       </c>
-      <c r="B332" s="12"/>
-      <c r="C332" s="12"/>
-      <c r="D332" s="12"/>
-      <c r="E332" s="12"/>
-      <c r="F332" s="12"/>
+      <c r="B332" s="16"/>
+      <c r="C332" s="16"/>
+      <c r="D332" s="16"/>
+      <c r="E332" s="16"/>
+      <c r="F332" s="16"/>
     </row>
     <row r="333" spans="1:6" ht="97.5" customHeight="1">
       <c r="A333" s="13" t="s">
@@ -23389,14 +23389,14 @@
       <c r="F336" s="13"/>
     </row>
     <row r="337" spans="1:6" ht="54" customHeight="1">
-      <c r="A337" s="14" t="s">
+      <c r="A337" s="20" t="s">
         <v>615</v>
       </c>
-      <c r="B337" s="14"/>
-      <c r="C337" s="14"/>
-      <c r="D337" s="14"/>
-      <c r="E337" s="14"/>
-      <c r="F337" s="14"/>
+      <c r="B337" s="20"/>
+      <c r="C337" s="20"/>
+      <c r="D337" s="20"/>
+      <c r="E337" s="20"/>
+      <c r="F337" s="20"/>
     </row>
     <row r="338" spans="1:6" ht="34.5" customHeight="1">
       <c r="A338" s="13" t="s">
@@ -23409,14 +23409,14 @@
       <c r="F338" s="13"/>
     </row>
     <row r="339" spans="1:6" ht="75" customHeight="1">
-      <c r="A339" s="12" t="s">
+      <c r="A339" s="16" t="s">
         <v>606</v>
       </c>
-      <c r="B339" s="12"/>
-      <c r="C339" s="12"/>
-      <c r="D339" s="12"/>
-      <c r="E339" s="12"/>
-      <c r="F339" s="12"/>
+      <c r="B339" s="16"/>
+      <c r="C339" s="16"/>
+      <c r="D339" s="16"/>
+      <c r="E339" s="16"/>
+      <c r="F339" s="16"/>
     </row>
     <row r="340" spans="1:6" ht="34.5" customHeight="1">
       <c r="A340" s="13" t="s">
@@ -23429,14 +23429,14 @@
       <c r="F340" s="13"/>
     </row>
     <row r="341" spans="1:6" ht="75" customHeight="1">
-      <c r="A341" s="12" t="s">
+      <c r="A341" s="16" t="s">
         <v>606</v>
       </c>
-      <c r="B341" s="12"/>
-      <c r="C341" s="12"/>
-      <c r="D341" s="12"/>
-      <c r="E341" s="12"/>
-      <c r="F341" s="12"/>
+      <c r="B341" s="16"/>
+      <c r="C341" s="16"/>
+      <c r="D341" s="16"/>
+      <c r="E341" s="16"/>
+      <c r="F341" s="16"/>
     </row>
     <row r="342" spans="1:6" ht="66" customHeight="1">
       <c r="A342" s="13" t="s">
@@ -23459,14 +23459,14 @@
       <c r="F343" s="13"/>
     </row>
     <row r="344" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A344" s="14" t="s">
+      <c r="A344" s="20" t="s">
         <v>620</v>
       </c>
-      <c r="B344" s="14"/>
-      <c r="C344" s="14"/>
-      <c r="D344" s="14"/>
-      <c r="E344" s="14"/>
-      <c r="F344" s="14"/>
+      <c r="B344" s="20"/>
+      <c r="C344" s="20"/>
+      <c r="D344" s="20"/>
+      <c r="E344" s="20"/>
+      <c r="F344" s="20"/>
     </row>
     <row r="345" spans="1:6" ht="55.5" customHeight="1">
       <c r="A345" s="13" t="s">
@@ -23489,14 +23489,14 @@
       <c r="F346" s="13"/>
     </row>
     <row r="347" spans="1:6" ht="75" customHeight="1">
-      <c r="A347" s="12" t="s">
+      <c r="A347" s="16" t="s">
         <v>623</v>
       </c>
-      <c r="B347" s="12"/>
-      <c r="C347" s="12"/>
-      <c r="D347" s="12"/>
-      <c r="E347" s="12"/>
-      <c r="F347" s="12"/>
+      <c r="B347" s="16"/>
+      <c r="C347" s="16"/>
+      <c r="D347" s="16"/>
+      <c r="E347" s="16"/>
+      <c r="F347" s="16"/>
     </row>
     <row r="348" spans="1:6" ht="76.5" customHeight="1">
       <c r="A348" s="13" t="s">
@@ -23529,14 +23529,14 @@
       <c r="F350" s="13"/>
     </row>
     <row r="351" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A351" s="14" t="s">
+      <c r="A351" s="20" t="s">
         <v>627</v>
       </c>
-      <c r="B351" s="14"/>
-      <c r="C351" s="14"/>
-      <c r="D351" s="14"/>
-      <c r="E351" s="14"/>
-      <c r="F351" s="14"/>
+      <c r="B351" s="20"/>
+      <c r="C351" s="20"/>
+      <c r="D351" s="20"/>
+      <c r="E351" s="20"/>
+      <c r="F351" s="20"/>
     </row>
     <row r="352" spans="1:6" ht="66" customHeight="1">
       <c r="A352" s="13" t="s">
@@ -23649,14 +23649,14 @@
       <c r="F362" s="13"/>
     </row>
     <row r="363" spans="1:6" ht="64.5" customHeight="1">
-      <c r="A363" s="14" t="s">
+      <c r="A363" s="20" t="s">
         <v>639</v>
       </c>
-      <c r="B363" s="14"/>
-      <c r="C363" s="14"/>
-      <c r="D363" s="14"/>
-      <c r="E363" s="14"/>
-      <c r="F363" s="14"/>
+      <c r="B363" s="20"/>
+      <c r="C363" s="20"/>
+      <c r="D363" s="20"/>
+      <c r="E363" s="20"/>
+      <c r="F363" s="20"/>
     </row>
     <row r="364" spans="1:6" ht="55.5" customHeight="1">
       <c r="A364" s="13" t="s">
@@ -23669,14 +23669,14 @@
       <c r="F364" s="13"/>
     </row>
     <row r="365" spans="1:6" ht="85.5" customHeight="1">
-      <c r="A365" s="12" t="s">
+      <c r="A365" s="16" t="s">
         <v>641</v>
       </c>
-      <c r="B365" s="12"/>
-      <c r="C365" s="12"/>
-      <c r="D365" s="12"/>
-      <c r="E365" s="12"/>
-      <c r="F365" s="12"/>
+      <c r="B365" s="16"/>
+      <c r="C365" s="16"/>
+      <c r="D365" s="16"/>
+      <c r="E365" s="16"/>
+      <c r="F365" s="16"/>
     </row>
     <row r="366" spans="1:6" ht="108" customHeight="1">
       <c r="A366" s="13" t="s">
@@ -23699,14 +23699,14 @@
       <c r="F367" s="13"/>
     </row>
     <row r="368" spans="1:6" ht="85.5" customHeight="1">
-      <c r="A368" s="12" t="s">
+      <c r="A368" s="16" t="s">
         <v>641</v>
       </c>
-      <c r="B368" s="12"/>
-      <c r="C368" s="12"/>
-      <c r="D368" s="12"/>
-      <c r="E368" s="12"/>
-      <c r="F368" s="12"/>
+      <c r="B368" s="16"/>
+      <c r="C368" s="16"/>
+      <c r="D368" s="16"/>
+      <c r="E368" s="16"/>
+      <c r="F368" s="16"/>
     </row>
     <row r="369" spans="1:6" ht="108" customHeight="1">
       <c r="A369" s="13" t="s">
@@ -23729,14 +23729,14 @@
       <c r="F370" s="13"/>
     </row>
     <row r="371" spans="1:6" ht="54" customHeight="1">
-      <c r="A371" s="12" t="s">
+      <c r="A371" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B371" s="12"/>
-      <c r="C371" s="12"/>
-      <c r="D371" s="12"/>
-      <c r="E371" s="12"/>
-      <c r="F371" s="12"/>
+      <c r="B371" s="16"/>
+      <c r="C371" s="16"/>
+      <c r="D371" s="16"/>
+      <c r="E371" s="16"/>
+      <c r="F371" s="16"/>
     </row>
     <row r="372" spans="1:6" ht="76.5" customHeight="1">
       <c r="A372" s="13" t="s">
@@ -23759,14 +23759,14 @@
       <c r="F373" s="13"/>
     </row>
     <row r="374" spans="1:6" ht="54" customHeight="1">
-      <c r="A374" s="12" t="s">
+      <c r="A374" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B374" s="12"/>
-      <c r="C374" s="12"/>
-      <c r="D374" s="12"/>
-      <c r="E374" s="12"/>
-      <c r="F374" s="12"/>
+      <c r="B374" s="16"/>
+      <c r="C374" s="16"/>
+      <c r="D374" s="16"/>
+      <c r="E374" s="16"/>
+      <c r="F374" s="16"/>
     </row>
     <row r="375" spans="1:6" ht="66" customHeight="1">
       <c r="A375" s="13" t="s">
@@ -23779,14 +23779,14 @@
       <c r="F375" s="13"/>
     </row>
     <row r="376" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A376" s="14" t="s">
+      <c r="A376" s="20" t="s">
         <v>650</v>
       </c>
-      <c r="B376" s="14"/>
-      <c r="C376" s="14"/>
-      <c r="D376" s="14"/>
-      <c r="E376" s="14"/>
-      <c r="F376" s="14"/>
+      <c r="B376" s="20"/>
+      <c r="C376" s="20"/>
+      <c r="D376" s="20"/>
+      <c r="E376" s="20"/>
+      <c r="F376" s="20"/>
     </row>
     <row r="377" spans="1:6" ht="76.5" customHeight="1">
       <c r="A377" s="13" t="s">
@@ -23809,14 +23809,14 @@
       <c r="F378" s="13"/>
     </row>
     <row r="379" spans="1:6" ht="54" customHeight="1">
-      <c r="A379" s="12" t="s">
+      <c r="A379" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B379" s="12"/>
-      <c r="C379" s="12"/>
-      <c r="D379" s="12"/>
-      <c r="E379" s="12"/>
-      <c r="F379" s="12"/>
+      <c r="B379" s="16"/>
+      <c r="C379" s="16"/>
+      <c r="D379" s="16"/>
+      <c r="E379" s="16"/>
+      <c r="F379" s="16"/>
     </row>
     <row r="380" spans="1:6" ht="45" customHeight="1">
       <c r="A380" s="13" t="s">
@@ -23829,14 +23829,14 @@
       <c r="F380" s="13"/>
     </row>
     <row r="381" spans="1:6" ht="54" customHeight="1">
-      <c r="A381" s="12" t="s">
+      <c r="A381" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B381" s="12"/>
-      <c r="C381" s="12"/>
-      <c r="D381" s="12"/>
-      <c r="E381" s="12"/>
-      <c r="F381" s="12"/>
+      <c r="B381" s="16"/>
+      <c r="C381" s="16"/>
+      <c r="D381" s="16"/>
+      <c r="E381" s="16"/>
+      <c r="F381" s="16"/>
     </row>
     <row r="382" spans="1:6" ht="76.5" customHeight="1">
       <c r="A382" s="13" t="s">
@@ -23879,14 +23879,14 @@
       <c r="F385" s="13"/>
     </row>
     <row r="386" spans="1:6" ht="54" customHeight="1">
-      <c r="A386" s="12" t="s">
+      <c r="A386" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B386" s="12"/>
-      <c r="C386" s="12"/>
-      <c r="D386" s="12"/>
-      <c r="E386" s="12"/>
-      <c r="F386" s="12"/>
+      <c r="B386" s="16"/>
+      <c r="C386" s="16"/>
+      <c r="D386" s="16"/>
+      <c r="E386" s="16"/>
+      <c r="F386" s="16"/>
     </row>
     <row r="387" spans="1:6" ht="76.5" customHeight="1">
       <c r="A387" s="13" t="s">
@@ -23919,14 +23919,14 @@
       <c r="F389" s="13"/>
     </row>
     <row r="390" spans="1:6" ht="54" customHeight="1">
-      <c r="A390" s="12" t="s">
+      <c r="A390" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B390" s="12"/>
-      <c r="C390" s="12"/>
-      <c r="D390" s="12"/>
-      <c r="E390" s="12"/>
-      <c r="F390" s="12"/>
+      <c r="B390" s="16"/>
+      <c r="C390" s="16"/>
+      <c r="D390" s="16"/>
+      <c r="E390" s="16"/>
+      <c r="F390" s="16"/>
     </row>
     <row r="391" spans="1:6" ht="34.5" customHeight="1">
       <c r="A391" s="13" t="s">
@@ -23939,14 +23939,14 @@
       <c r="F391" s="13"/>
     </row>
     <row r="392" spans="1:6" ht="54" customHeight="1">
-      <c r="A392" s="12" t="s">
+      <c r="A392" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B392" s="12"/>
-      <c r="C392" s="12"/>
-      <c r="D392" s="12"/>
-      <c r="E392" s="12"/>
-      <c r="F392" s="12"/>
+      <c r="B392" s="16"/>
+      <c r="C392" s="16"/>
+      <c r="D392" s="16"/>
+      <c r="E392" s="16"/>
+      <c r="F392" s="16"/>
     </row>
     <row r="393" spans="1:6" ht="34.5" customHeight="1">
       <c r="A393" s="13" t="s">
@@ -23959,14 +23959,14 @@
       <c r="F393" s="13"/>
     </row>
     <row r="394" spans="1:6" ht="54" customHeight="1">
-      <c r="A394" s="12" t="s">
+      <c r="A394" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B394" s="12"/>
-      <c r="C394" s="12"/>
-      <c r="D394" s="12"/>
-      <c r="E394" s="12"/>
-      <c r="F394" s="12"/>
+      <c r="B394" s="16"/>
+      <c r="C394" s="16"/>
+      <c r="D394" s="16"/>
+      <c r="E394" s="16"/>
+      <c r="F394" s="16"/>
     </row>
     <row r="395" spans="1:6" ht="34.5" customHeight="1">
       <c r="A395" s="13" t="s">
@@ -23979,14 +23979,14 @@
       <c r="F395" s="13"/>
     </row>
     <row r="396" spans="1:6" ht="54" customHeight="1">
-      <c r="A396" s="12" t="s">
+      <c r="A396" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B396" s="12"/>
-      <c r="C396" s="12"/>
-      <c r="D396" s="12"/>
-      <c r="E396" s="12"/>
-      <c r="F396" s="12"/>
+      <c r="B396" s="16"/>
+      <c r="C396" s="16"/>
+      <c r="D396" s="16"/>
+      <c r="E396" s="16"/>
+      <c r="F396" s="16"/>
     </row>
     <row r="397" spans="1:6" ht="76.5" customHeight="1">
       <c r="A397" s="13" t="s">
@@ -24009,14 +24009,14 @@
       <c r="F398" s="13"/>
     </row>
     <row r="399" spans="1:6" ht="54" customHeight="1">
-      <c r="A399" s="12" t="s">
+      <c r="A399" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B399" s="12"/>
-      <c r="C399" s="12"/>
-      <c r="D399" s="12"/>
-      <c r="E399" s="12"/>
-      <c r="F399" s="12"/>
+      <c r="B399" s="16"/>
+      <c r="C399" s="16"/>
+      <c r="D399" s="16"/>
+      <c r="E399" s="16"/>
+      <c r="F399" s="16"/>
     </row>
     <row r="400" spans="1:6" ht="34.5" customHeight="1">
       <c r="A400" s="13" t="s">
@@ -24029,14 +24029,14 @@
       <c r="F400" s="13"/>
     </row>
     <row r="401" spans="1:6" ht="54" customHeight="1">
-      <c r="A401" s="12" t="s">
+      <c r="A401" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B401" s="12"/>
-      <c r="C401" s="12"/>
-      <c r="D401" s="12"/>
-      <c r="E401" s="12"/>
-      <c r="F401" s="12"/>
+      <c r="B401" s="16"/>
+      <c r="C401" s="16"/>
+      <c r="D401" s="16"/>
+      <c r="E401" s="16"/>
+      <c r="F401" s="16"/>
     </row>
     <row r="402" spans="1:6" ht="76.5" customHeight="1">
       <c r="A402" s="13" t="s">
@@ -24069,14 +24069,14 @@
       <c r="F404" s="13"/>
     </row>
     <row r="405" spans="1:6" ht="54" customHeight="1">
-      <c r="A405" s="12" t="s">
+      <c r="A405" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B405" s="12"/>
-      <c r="C405" s="12"/>
-      <c r="D405" s="12"/>
-      <c r="E405" s="12"/>
-      <c r="F405" s="12"/>
+      <c r="B405" s="16"/>
+      <c r="C405" s="16"/>
+      <c r="D405" s="16"/>
+      <c r="E405" s="16"/>
+      <c r="F405" s="16"/>
     </row>
     <row r="406" spans="1:6" ht="76.5" customHeight="1">
       <c r="A406" s="13" t="s">
@@ -24109,14 +24109,14 @@
       <c r="F408" s="13"/>
     </row>
     <row r="409" spans="1:6" ht="54" customHeight="1">
-      <c r="A409" s="12" t="s">
+      <c r="A409" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B409" s="12"/>
-      <c r="C409" s="12"/>
-      <c r="D409" s="12"/>
-      <c r="E409" s="12"/>
-      <c r="F409" s="12"/>
+      <c r="B409" s="16"/>
+      <c r="C409" s="16"/>
+      <c r="D409" s="16"/>
+      <c r="E409" s="16"/>
+      <c r="F409" s="16"/>
     </row>
     <row r="410" spans="1:6" ht="34.5" customHeight="1">
       <c r="A410" s="13" t="s">
@@ -24129,14 +24129,14 @@
       <c r="F410" s="13"/>
     </row>
     <row r="411" spans="1:6" ht="54" customHeight="1">
-      <c r="A411" s="12" t="s">
+      <c r="A411" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="B411" s="12"/>
-      <c r="C411" s="12"/>
-      <c r="D411" s="12"/>
-      <c r="E411" s="12"/>
-      <c r="F411" s="12"/>
+      <c r="B411" s="16"/>
+      <c r="C411" s="16"/>
+      <c r="D411" s="16"/>
+      <c r="E411" s="16"/>
+      <c r="F411" s="16"/>
     </row>
     <row r="412" spans="1:6" ht="34.5" customHeight="1">
       <c r="A412" s="13" t="s">
@@ -24169,24 +24169,24 @@
       <c r="F414" s="13"/>
     </row>
     <row r="415" spans="1:6" ht="33" customHeight="1">
-      <c r="A415" s="12" t="s">
+      <c r="A415" s="16" t="s">
         <v>677</v>
       </c>
-      <c r="B415" s="12"/>
-      <c r="C415" s="12"/>
-      <c r="D415" s="12"/>
-      <c r="E415" s="12"/>
-      <c r="F415" s="12"/>
+      <c r="B415" s="16"/>
+      <c r="C415" s="16"/>
+      <c r="D415" s="16"/>
+      <c r="E415" s="16"/>
+      <c r="F415" s="16"/>
     </row>
     <row r="416" spans="1:6" ht="64.5" customHeight="1">
-      <c r="A416" s="12" t="s">
+      <c r="A416" s="16" t="s">
         <v>678</v>
       </c>
-      <c r="B416" s="12"/>
-      <c r="C416" s="12"/>
-      <c r="D416" s="12"/>
-      <c r="E416" s="12"/>
-      <c r="F416" s="12"/>
+      <c r="B416" s="16"/>
+      <c r="C416" s="16"/>
+      <c r="D416" s="16"/>
+      <c r="E416" s="16"/>
+      <c r="F416" s="16"/>
     </row>
     <row r="417" spans="1:6" ht="34.5" customHeight="1">
       <c r="A417" s="13" t="s">
@@ -24199,14 +24199,14 @@
       <c r="F417" s="13"/>
     </row>
     <row r="418" spans="1:6" ht="54" customHeight="1">
-      <c r="A418" s="12" t="s">
+      <c r="A418" s="16" t="s">
         <v>680</v>
       </c>
-      <c r="B418" s="12"/>
-      <c r="C418" s="12"/>
-      <c r="D418" s="12"/>
-      <c r="E418" s="12"/>
-      <c r="F418" s="12"/>
+      <c r="B418" s="16"/>
+      <c r="C418" s="16"/>
+      <c r="D418" s="16"/>
+      <c r="E418" s="16"/>
+      <c r="F418" s="16"/>
     </row>
     <row r="419" spans="1:6" ht="222.75" customHeight="1">
       <c r="A419" s="13" t="s">
@@ -24230,411 +24230,6 @@
     </row>
   </sheetData>
   <mergeCells count="420">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A49:F49"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A59:F59"/>
-    <mergeCell ref="A60:F60"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A64:F64"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A66:F66"/>
-    <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="A71:F71"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A73:F73"/>
-    <mergeCell ref="A74:F74"/>
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="A76:F76"/>
-    <mergeCell ref="A77:F77"/>
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A79:F79"/>
-    <mergeCell ref="A80:F80"/>
-    <mergeCell ref="A81:F81"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A83:F83"/>
-    <mergeCell ref="A84:F84"/>
-    <mergeCell ref="A85:F85"/>
-    <mergeCell ref="A86:F86"/>
-    <mergeCell ref="A87:F87"/>
-    <mergeCell ref="A88:F88"/>
-    <mergeCell ref="A89:F89"/>
-    <mergeCell ref="A90:F90"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A92:F92"/>
-    <mergeCell ref="A93:F93"/>
-    <mergeCell ref="A94:F94"/>
-    <mergeCell ref="A95:F95"/>
-    <mergeCell ref="A96:F96"/>
-    <mergeCell ref="A97:F97"/>
-    <mergeCell ref="A98:F98"/>
-    <mergeCell ref="A99:F99"/>
-    <mergeCell ref="A100:F100"/>
-    <mergeCell ref="A101:F101"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A103:F103"/>
-    <mergeCell ref="A104:F104"/>
-    <mergeCell ref="A105:F105"/>
-    <mergeCell ref="A106:F106"/>
-    <mergeCell ref="A107:F107"/>
-    <mergeCell ref="A108:F108"/>
-    <mergeCell ref="A109:F109"/>
-    <mergeCell ref="A110:F110"/>
-    <mergeCell ref="A111:F111"/>
-    <mergeCell ref="A112:F112"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A114:F114"/>
-    <mergeCell ref="A115:F115"/>
-    <mergeCell ref="A116:F116"/>
-    <mergeCell ref="A117:F117"/>
-    <mergeCell ref="A118:F118"/>
-    <mergeCell ref="A119:F119"/>
-    <mergeCell ref="A120:F120"/>
-    <mergeCell ref="A121:F121"/>
-    <mergeCell ref="A122:F122"/>
-    <mergeCell ref="A123:F123"/>
-    <mergeCell ref="A124:F124"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="A126:F126"/>
-    <mergeCell ref="A127:F127"/>
-    <mergeCell ref="A128:F128"/>
-    <mergeCell ref="A129:F129"/>
-    <mergeCell ref="A130:F130"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="A132:F132"/>
-    <mergeCell ref="A133:F133"/>
-    <mergeCell ref="A134:F134"/>
-    <mergeCell ref="A135:F135"/>
-    <mergeCell ref="A136:F136"/>
-    <mergeCell ref="A137:F137"/>
-    <mergeCell ref="A138:F138"/>
-    <mergeCell ref="A139:F139"/>
-    <mergeCell ref="A140:F140"/>
-    <mergeCell ref="A141:F141"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A143:F143"/>
-    <mergeCell ref="A144:F144"/>
-    <mergeCell ref="A145:F145"/>
-    <mergeCell ref="A146:F146"/>
-    <mergeCell ref="A147:F147"/>
-    <mergeCell ref="A148:F148"/>
-    <mergeCell ref="A149:F149"/>
-    <mergeCell ref="A150:F150"/>
-    <mergeCell ref="A151:F151"/>
-    <mergeCell ref="A152:F152"/>
-    <mergeCell ref="A153:F153"/>
-    <mergeCell ref="A154:F154"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A156:F156"/>
-    <mergeCell ref="A157:F157"/>
-    <mergeCell ref="A158:F158"/>
-    <mergeCell ref="A159:F159"/>
-    <mergeCell ref="A160:F160"/>
-    <mergeCell ref="A161:F161"/>
-    <mergeCell ref="A162:F162"/>
-    <mergeCell ref="A163:F163"/>
-    <mergeCell ref="A164:F164"/>
-    <mergeCell ref="A165:F165"/>
-    <mergeCell ref="A166:F166"/>
-    <mergeCell ref="A167:F167"/>
-    <mergeCell ref="A168:F168"/>
-    <mergeCell ref="A169:F169"/>
-    <mergeCell ref="A170:F170"/>
-    <mergeCell ref="A171:F171"/>
-    <mergeCell ref="A172:F172"/>
-    <mergeCell ref="A173:F173"/>
-    <mergeCell ref="A174:F174"/>
-    <mergeCell ref="A175:F175"/>
-    <mergeCell ref="A176:F176"/>
-    <mergeCell ref="A177:F177"/>
-    <mergeCell ref="A178:F178"/>
-    <mergeCell ref="A179:F179"/>
-    <mergeCell ref="A180:F180"/>
-    <mergeCell ref="A181:F181"/>
-    <mergeCell ref="A182:F182"/>
-    <mergeCell ref="A183:F183"/>
-    <mergeCell ref="A184:F184"/>
-    <mergeCell ref="A185:F185"/>
-    <mergeCell ref="A186:F186"/>
-    <mergeCell ref="A187:F187"/>
-    <mergeCell ref="A188:F188"/>
-    <mergeCell ref="A189:F189"/>
-    <mergeCell ref="A190:F190"/>
-    <mergeCell ref="A191:F191"/>
-    <mergeCell ref="A192:F192"/>
-    <mergeCell ref="A193:F193"/>
-    <mergeCell ref="A194:F194"/>
-    <mergeCell ref="A195:F195"/>
-    <mergeCell ref="A196:F196"/>
-    <mergeCell ref="A197:F197"/>
-    <mergeCell ref="A198:F198"/>
-    <mergeCell ref="A199:F199"/>
-    <mergeCell ref="A200:F200"/>
-    <mergeCell ref="A201:F201"/>
-    <mergeCell ref="A202:F202"/>
-    <mergeCell ref="A203:F203"/>
-    <mergeCell ref="A204:F204"/>
-    <mergeCell ref="A205:F205"/>
-    <mergeCell ref="A206:F206"/>
-    <mergeCell ref="A207:F207"/>
-    <mergeCell ref="A208:F208"/>
-    <mergeCell ref="A209:F209"/>
-    <mergeCell ref="A210:F210"/>
-    <mergeCell ref="A211:F211"/>
-    <mergeCell ref="A212:F212"/>
-    <mergeCell ref="A213:F213"/>
-    <mergeCell ref="A214:F214"/>
-    <mergeCell ref="A215:F215"/>
-    <mergeCell ref="A216:F216"/>
-    <mergeCell ref="A217:F217"/>
-    <mergeCell ref="A218:F218"/>
-    <mergeCell ref="A219:F219"/>
-    <mergeCell ref="A220:F220"/>
-    <mergeCell ref="A221:F221"/>
-    <mergeCell ref="A222:F222"/>
-    <mergeCell ref="A223:F223"/>
-    <mergeCell ref="A224:F224"/>
-    <mergeCell ref="A225:F225"/>
-    <mergeCell ref="A226:F226"/>
-    <mergeCell ref="A227:F227"/>
-    <mergeCell ref="A228:F228"/>
-    <mergeCell ref="A229:F229"/>
-    <mergeCell ref="A230:F230"/>
-    <mergeCell ref="A231:F231"/>
-    <mergeCell ref="A232:F232"/>
-    <mergeCell ref="A233:F233"/>
-    <mergeCell ref="A234:F234"/>
-    <mergeCell ref="A235:F235"/>
-    <mergeCell ref="A236:F236"/>
-    <mergeCell ref="A237:F237"/>
-    <mergeCell ref="A238:F238"/>
-    <mergeCell ref="A239:F239"/>
-    <mergeCell ref="A240:F240"/>
-    <mergeCell ref="A241:F241"/>
-    <mergeCell ref="A242:F242"/>
-    <mergeCell ref="A243:F243"/>
-    <mergeCell ref="A244:F244"/>
-    <mergeCell ref="A245:F245"/>
-    <mergeCell ref="A246:F246"/>
-    <mergeCell ref="A247:F247"/>
-    <mergeCell ref="A248:F248"/>
-    <mergeCell ref="A249:F249"/>
-    <mergeCell ref="A250:F250"/>
-    <mergeCell ref="A251:F251"/>
-    <mergeCell ref="A252:F252"/>
-    <mergeCell ref="A253:F253"/>
-    <mergeCell ref="A254:F254"/>
-    <mergeCell ref="A255:F255"/>
-    <mergeCell ref="A256:F256"/>
-    <mergeCell ref="A257:F257"/>
-    <mergeCell ref="A258:F258"/>
-    <mergeCell ref="A259:F259"/>
-    <mergeCell ref="A260:F260"/>
-    <mergeCell ref="A261:F261"/>
-    <mergeCell ref="A262:F262"/>
-    <mergeCell ref="A263:F263"/>
-    <mergeCell ref="A264:F264"/>
-    <mergeCell ref="A265:F265"/>
-    <mergeCell ref="A266:F266"/>
-    <mergeCell ref="A267:F267"/>
-    <mergeCell ref="A268:F268"/>
-    <mergeCell ref="A269:F269"/>
-    <mergeCell ref="A270:F270"/>
-    <mergeCell ref="A271:F271"/>
-    <mergeCell ref="A272:F272"/>
-    <mergeCell ref="A273:F273"/>
-    <mergeCell ref="A274:F274"/>
-    <mergeCell ref="A275:F275"/>
-    <mergeCell ref="A276:F276"/>
-    <mergeCell ref="A277:F277"/>
-    <mergeCell ref="A278:F278"/>
-    <mergeCell ref="A279:F279"/>
-    <mergeCell ref="A280:F280"/>
-    <mergeCell ref="A281:F281"/>
-    <mergeCell ref="A282:F282"/>
-    <mergeCell ref="A283:F283"/>
-    <mergeCell ref="A284:F284"/>
-    <mergeCell ref="A285:F285"/>
-    <mergeCell ref="A286:F286"/>
-    <mergeCell ref="A287:F287"/>
-    <mergeCell ref="A288:F288"/>
-    <mergeCell ref="A289:F289"/>
-    <mergeCell ref="A290:F290"/>
-    <mergeCell ref="A291:F291"/>
-    <mergeCell ref="A292:F292"/>
-    <mergeCell ref="A293:F293"/>
-    <mergeCell ref="A294:F294"/>
-    <mergeCell ref="A295:F295"/>
-    <mergeCell ref="A296:F296"/>
-    <mergeCell ref="A297:F297"/>
-    <mergeCell ref="A298:F298"/>
-    <mergeCell ref="A299:F299"/>
-    <mergeCell ref="A300:F300"/>
-    <mergeCell ref="A301:F301"/>
-    <mergeCell ref="A302:F302"/>
-    <mergeCell ref="A303:F303"/>
-    <mergeCell ref="A304:F304"/>
-    <mergeCell ref="A305:F305"/>
-    <mergeCell ref="A306:F306"/>
-    <mergeCell ref="A307:F307"/>
-    <mergeCell ref="A308:F308"/>
-    <mergeCell ref="A309:F309"/>
-    <mergeCell ref="A310:F310"/>
-    <mergeCell ref="A311:F311"/>
-    <mergeCell ref="A312:F312"/>
-    <mergeCell ref="A313:F313"/>
-    <mergeCell ref="A314:F314"/>
-    <mergeCell ref="A315:F315"/>
-    <mergeCell ref="A316:F316"/>
-    <mergeCell ref="A317:F317"/>
-    <mergeCell ref="A318:F318"/>
-    <mergeCell ref="A319:F319"/>
-    <mergeCell ref="A320:F320"/>
-    <mergeCell ref="A321:F321"/>
-    <mergeCell ref="A322:F322"/>
-    <mergeCell ref="A323:F323"/>
-    <mergeCell ref="A324:F324"/>
-    <mergeCell ref="A325:F325"/>
-    <mergeCell ref="A326:F326"/>
-    <mergeCell ref="A327:F327"/>
-    <mergeCell ref="A328:F328"/>
-    <mergeCell ref="A329:F329"/>
-    <mergeCell ref="A330:F330"/>
-    <mergeCell ref="A331:F331"/>
-    <mergeCell ref="A332:F332"/>
-    <mergeCell ref="A333:F333"/>
-    <mergeCell ref="A334:F334"/>
-    <mergeCell ref="A335:F335"/>
-    <mergeCell ref="A336:F336"/>
-    <mergeCell ref="A337:F337"/>
-    <mergeCell ref="A338:F338"/>
-    <mergeCell ref="A339:F339"/>
-    <mergeCell ref="A340:F340"/>
-    <mergeCell ref="A341:F341"/>
-    <mergeCell ref="A342:F342"/>
-    <mergeCell ref="A343:F343"/>
-    <mergeCell ref="A344:F344"/>
-    <mergeCell ref="A345:F345"/>
-    <mergeCell ref="A346:F346"/>
-    <mergeCell ref="A347:F347"/>
-    <mergeCell ref="A348:F348"/>
-    <mergeCell ref="A349:F349"/>
-    <mergeCell ref="A350:F350"/>
-    <mergeCell ref="A351:F351"/>
-    <mergeCell ref="A352:F352"/>
-    <mergeCell ref="A353:F353"/>
-    <mergeCell ref="A354:F354"/>
-    <mergeCell ref="A355:F355"/>
-    <mergeCell ref="A356:F356"/>
-    <mergeCell ref="A357:F357"/>
-    <mergeCell ref="A358:F358"/>
-    <mergeCell ref="A359:F359"/>
-    <mergeCell ref="A360:F360"/>
-    <mergeCell ref="A361:F361"/>
-    <mergeCell ref="A362:F362"/>
-    <mergeCell ref="A363:F363"/>
-    <mergeCell ref="A364:F364"/>
-    <mergeCell ref="A365:F365"/>
-    <mergeCell ref="A366:F366"/>
-    <mergeCell ref="A367:F367"/>
-    <mergeCell ref="A368:F368"/>
-    <mergeCell ref="A369:F369"/>
-    <mergeCell ref="A370:F370"/>
-    <mergeCell ref="A371:F371"/>
-    <mergeCell ref="A372:F372"/>
-    <mergeCell ref="A373:F373"/>
-    <mergeCell ref="A374:F374"/>
-    <mergeCell ref="A375:F375"/>
-    <mergeCell ref="A376:F376"/>
-    <mergeCell ref="A377:F377"/>
-    <mergeCell ref="A378:F378"/>
-    <mergeCell ref="A379:F379"/>
-    <mergeCell ref="A380:F380"/>
-    <mergeCell ref="A381:F381"/>
-    <mergeCell ref="A382:F382"/>
-    <mergeCell ref="A383:F383"/>
-    <mergeCell ref="A384:F384"/>
-    <mergeCell ref="A385:F385"/>
-    <mergeCell ref="A386:F386"/>
-    <mergeCell ref="A387:F387"/>
-    <mergeCell ref="A388:F388"/>
-    <mergeCell ref="A389:F389"/>
-    <mergeCell ref="A390:F390"/>
-    <mergeCell ref="A391:F391"/>
-    <mergeCell ref="A392:F392"/>
-    <mergeCell ref="A393:F393"/>
-    <mergeCell ref="A394:F394"/>
-    <mergeCell ref="A395:F395"/>
-    <mergeCell ref="A396:F396"/>
-    <mergeCell ref="A397:F397"/>
-    <mergeCell ref="A398:F398"/>
-    <mergeCell ref="A399:F399"/>
-    <mergeCell ref="A400:F400"/>
-    <mergeCell ref="A401:F401"/>
-    <mergeCell ref="A402:F402"/>
-    <mergeCell ref="A403:F403"/>
-    <mergeCell ref="A404:F404"/>
-    <mergeCell ref="A405:F405"/>
     <mergeCell ref="A415:F415"/>
     <mergeCell ref="A416:F416"/>
     <mergeCell ref="A417:F417"/>
@@ -24650,6 +24245,411 @@
     <mergeCell ref="A412:F412"/>
     <mergeCell ref="A413:F413"/>
     <mergeCell ref="A414:F414"/>
+    <mergeCell ref="A397:F397"/>
+    <mergeCell ref="A398:F398"/>
+    <mergeCell ref="A399:F399"/>
+    <mergeCell ref="A400:F400"/>
+    <mergeCell ref="A401:F401"/>
+    <mergeCell ref="A402:F402"/>
+    <mergeCell ref="A403:F403"/>
+    <mergeCell ref="A404:F404"/>
+    <mergeCell ref="A405:F405"/>
+    <mergeCell ref="A388:F388"/>
+    <mergeCell ref="A389:F389"/>
+    <mergeCell ref="A390:F390"/>
+    <mergeCell ref="A391:F391"/>
+    <mergeCell ref="A392:F392"/>
+    <mergeCell ref="A393:F393"/>
+    <mergeCell ref="A394:F394"/>
+    <mergeCell ref="A395:F395"/>
+    <mergeCell ref="A396:F396"/>
+    <mergeCell ref="A379:F379"/>
+    <mergeCell ref="A380:F380"/>
+    <mergeCell ref="A381:F381"/>
+    <mergeCell ref="A382:F382"/>
+    <mergeCell ref="A383:F383"/>
+    <mergeCell ref="A384:F384"/>
+    <mergeCell ref="A385:F385"/>
+    <mergeCell ref="A386:F386"/>
+    <mergeCell ref="A387:F387"/>
+    <mergeCell ref="A370:F370"/>
+    <mergeCell ref="A371:F371"/>
+    <mergeCell ref="A372:F372"/>
+    <mergeCell ref="A373:F373"/>
+    <mergeCell ref="A374:F374"/>
+    <mergeCell ref="A375:F375"/>
+    <mergeCell ref="A376:F376"/>
+    <mergeCell ref="A377:F377"/>
+    <mergeCell ref="A378:F378"/>
+    <mergeCell ref="A361:F361"/>
+    <mergeCell ref="A362:F362"/>
+    <mergeCell ref="A363:F363"/>
+    <mergeCell ref="A364:F364"/>
+    <mergeCell ref="A365:F365"/>
+    <mergeCell ref="A366:F366"/>
+    <mergeCell ref="A367:F367"/>
+    <mergeCell ref="A368:F368"/>
+    <mergeCell ref="A369:F369"/>
+    <mergeCell ref="A352:F352"/>
+    <mergeCell ref="A353:F353"/>
+    <mergeCell ref="A354:F354"/>
+    <mergeCell ref="A355:F355"/>
+    <mergeCell ref="A356:F356"/>
+    <mergeCell ref="A357:F357"/>
+    <mergeCell ref="A358:F358"/>
+    <mergeCell ref="A359:F359"/>
+    <mergeCell ref="A360:F360"/>
+    <mergeCell ref="A343:F343"/>
+    <mergeCell ref="A344:F344"/>
+    <mergeCell ref="A345:F345"/>
+    <mergeCell ref="A346:F346"/>
+    <mergeCell ref="A347:F347"/>
+    <mergeCell ref="A348:F348"/>
+    <mergeCell ref="A349:F349"/>
+    <mergeCell ref="A350:F350"/>
+    <mergeCell ref="A351:F351"/>
+    <mergeCell ref="A334:F334"/>
+    <mergeCell ref="A335:F335"/>
+    <mergeCell ref="A336:F336"/>
+    <mergeCell ref="A337:F337"/>
+    <mergeCell ref="A338:F338"/>
+    <mergeCell ref="A339:F339"/>
+    <mergeCell ref="A340:F340"/>
+    <mergeCell ref="A341:F341"/>
+    <mergeCell ref="A342:F342"/>
+    <mergeCell ref="A325:F325"/>
+    <mergeCell ref="A326:F326"/>
+    <mergeCell ref="A327:F327"/>
+    <mergeCell ref="A328:F328"/>
+    <mergeCell ref="A329:F329"/>
+    <mergeCell ref="A330:F330"/>
+    <mergeCell ref="A331:F331"/>
+    <mergeCell ref="A332:F332"/>
+    <mergeCell ref="A333:F333"/>
+    <mergeCell ref="A316:F316"/>
+    <mergeCell ref="A317:F317"/>
+    <mergeCell ref="A318:F318"/>
+    <mergeCell ref="A319:F319"/>
+    <mergeCell ref="A320:F320"/>
+    <mergeCell ref="A321:F321"/>
+    <mergeCell ref="A322:F322"/>
+    <mergeCell ref="A323:F323"/>
+    <mergeCell ref="A324:F324"/>
+    <mergeCell ref="A307:F307"/>
+    <mergeCell ref="A308:F308"/>
+    <mergeCell ref="A309:F309"/>
+    <mergeCell ref="A310:F310"/>
+    <mergeCell ref="A311:F311"/>
+    <mergeCell ref="A312:F312"/>
+    <mergeCell ref="A313:F313"/>
+    <mergeCell ref="A314:F314"/>
+    <mergeCell ref="A315:F315"/>
+    <mergeCell ref="A298:F298"/>
+    <mergeCell ref="A299:F299"/>
+    <mergeCell ref="A300:F300"/>
+    <mergeCell ref="A301:F301"/>
+    <mergeCell ref="A302:F302"/>
+    <mergeCell ref="A303:F303"/>
+    <mergeCell ref="A304:F304"/>
+    <mergeCell ref="A305:F305"/>
+    <mergeCell ref="A306:F306"/>
+    <mergeCell ref="A289:F289"/>
+    <mergeCell ref="A290:F290"/>
+    <mergeCell ref="A291:F291"/>
+    <mergeCell ref="A292:F292"/>
+    <mergeCell ref="A293:F293"/>
+    <mergeCell ref="A294:F294"/>
+    <mergeCell ref="A295:F295"/>
+    <mergeCell ref="A296:F296"/>
+    <mergeCell ref="A297:F297"/>
+    <mergeCell ref="A280:F280"/>
+    <mergeCell ref="A281:F281"/>
+    <mergeCell ref="A282:F282"/>
+    <mergeCell ref="A283:F283"/>
+    <mergeCell ref="A284:F284"/>
+    <mergeCell ref="A285:F285"/>
+    <mergeCell ref="A286:F286"/>
+    <mergeCell ref="A287:F287"/>
+    <mergeCell ref="A288:F288"/>
+    <mergeCell ref="A271:F271"/>
+    <mergeCell ref="A272:F272"/>
+    <mergeCell ref="A273:F273"/>
+    <mergeCell ref="A274:F274"/>
+    <mergeCell ref="A275:F275"/>
+    <mergeCell ref="A276:F276"/>
+    <mergeCell ref="A277:F277"/>
+    <mergeCell ref="A278:F278"/>
+    <mergeCell ref="A279:F279"/>
+    <mergeCell ref="A262:F262"/>
+    <mergeCell ref="A263:F263"/>
+    <mergeCell ref="A264:F264"/>
+    <mergeCell ref="A265:F265"/>
+    <mergeCell ref="A266:F266"/>
+    <mergeCell ref="A267:F267"/>
+    <mergeCell ref="A268:F268"/>
+    <mergeCell ref="A269:F269"/>
+    <mergeCell ref="A270:F270"/>
+    <mergeCell ref="A253:F253"/>
+    <mergeCell ref="A254:F254"/>
+    <mergeCell ref="A255:F255"/>
+    <mergeCell ref="A256:F256"/>
+    <mergeCell ref="A257:F257"/>
+    <mergeCell ref="A258:F258"/>
+    <mergeCell ref="A259:F259"/>
+    <mergeCell ref="A260:F260"/>
+    <mergeCell ref="A261:F261"/>
+    <mergeCell ref="A244:F244"/>
+    <mergeCell ref="A245:F245"/>
+    <mergeCell ref="A246:F246"/>
+    <mergeCell ref="A247:F247"/>
+    <mergeCell ref="A248:F248"/>
+    <mergeCell ref="A249:F249"/>
+    <mergeCell ref="A250:F250"/>
+    <mergeCell ref="A251:F251"/>
+    <mergeCell ref="A252:F252"/>
+    <mergeCell ref="A235:F235"/>
+    <mergeCell ref="A236:F236"/>
+    <mergeCell ref="A237:F237"/>
+    <mergeCell ref="A238:F238"/>
+    <mergeCell ref="A239:F239"/>
+    <mergeCell ref="A240:F240"/>
+    <mergeCell ref="A241:F241"/>
+    <mergeCell ref="A242:F242"/>
+    <mergeCell ref="A243:F243"/>
+    <mergeCell ref="A226:F226"/>
+    <mergeCell ref="A227:F227"/>
+    <mergeCell ref="A228:F228"/>
+    <mergeCell ref="A229:F229"/>
+    <mergeCell ref="A230:F230"/>
+    <mergeCell ref="A231:F231"/>
+    <mergeCell ref="A232:F232"/>
+    <mergeCell ref="A233:F233"/>
+    <mergeCell ref="A234:F234"/>
+    <mergeCell ref="A217:F217"/>
+    <mergeCell ref="A218:F218"/>
+    <mergeCell ref="A219:F219"/>
+    <mergeCell ref="A220:F220"/>
+    <mergeCell ref="A221:F221"/>
+    <mergeCell ref="A222:F222"/>
+    <mergeCell ref="A223:F223"/>
+    <mergeCell ref="A224:F224"/>
+    <mergeCell ref="A225:F225"/>
+    <mergeCell ref="A208:F208"/>
+    <mergeCell ref="A209:F209"/>
+    <mergeCell ref="A210:F210"/>
+    <mergeCell ref="A211:F211"/>
+    <mergeCell ref="A212:F212"/>
+    <mergeCell ref="A213:F213"/>
+    <mergeCell ref="A214:F214"/>
+    <mergeCell ref="A215:F215"/>
+    <mergeCell ref="A216:F216"/>
+    <mergeCell ref="A199:F199"/>
+    <mergeCell ref="A200:F200"/>
+    <mergeCell ref="A201:F201"/>
+    <mergeCell ref="A202:F202"/>
+    <mergeCell ref="A203:F203"/>
+    <mergeCell ref="A204:F204"/>
+    <mergeCell ref="A205:F205"/>
+    <mergeCell ref="A206:F206"/>
+    <mergeCell ref="A207:F207"/>
+    <mergeCell ref="A190:F190"/>
+    <mergeCell ref="A191:F191"/>
+    <mergeCell ref="A192:F192"/>
+    <mergeCell ref="A193:F193"/>
+    <mergeCell ref="A194:F194"/>
+    <mergeCell ref="A195:F195"/>
+    <mergeCell ref="A196:F196"/>
+    <mergeCell ref="A197:F197"/>
+    <mergeCell ref="A198:F198"/>
+    <mergeCell ref="A181:F181"/>
+    <mergeCell ref="A182:F182"/>
+    <mergeCell ref="A183:F183"/>
+    <mergeCell ref="A184:F184"/>
+    <mergeCell ref="A185:F185"/>
+    <mergeCell ref="A186:F186"/>
+    <mergeCell ref="A187:F187"/>
+    <mergeCell ref="A188:F188"/>
+    <mergeCell ref="A189:F189"/>
+    <mergeCell ref="A172:F172"/>
+    <mergeCell ref="A173:F173"/>
+    <mergeCell ref="A174:F174"/>
+    <mergeCell ref="A175:F175"/>
+    <mergeCell ref="A176:F176"/>
+    <mergeCell ref="A177:F177"/>
+    <mergeCell ref="A178:F178"/>
+    <mergeCell ref="A179:F179"/>
+    <mergeCell ref="A180:F180"/>
+    <mergeCell ref="A163:F163"/>
+    <mergeCell ref="A164:F164"/>
+    <mergeCell ref="A165:F165"/>
+    <mergeCell ref="A166:F166"/>
+    <mergeCell ref="A167:F167"/>
+    <mergeCell ref="A168:F168"/>
+    <mergeCell ref="A169:F169"/>
+    <mergeCell ref="A170:F170"/>
+    <mergeCell ref="A171:F171"/>
+    <mergeCell ref="A154:F154"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A156:F156"/>
+    <mergeCell ref="A157:F157"/>
+    <mergeCell ref="A158:F158"/>
+    <mergeCell ref="A159:F159"/>
+    <mergeCell ref="A160:F160"/>
+    <mergeCell ref="A161:F161"/>
+    <mergeCell ref="A162:F162"/>
+    <mergeCell ref="A145:F145"/>
+    <mergeCell ref="A146:F146"/>
+    <mergeCell ref="A147:F147"/>
+    <mergeCell ref="A148:F148"/>
+    <mergeCell ref="A149:F149"/>
+    <mergeCell ref="A150:F150"/>
+    <mergeCell ref="A151:F151"/>
+    <mergeCell ref="A152:F152"/>
+    <mergeCell ref="A153:F153"/>
+    <mergeCell ref="A136:F136"/>
+    <mergeCell ref="A137:F137"/>
+    <mergeCell ref="A138:F138"/>
+    <mergeCell ref="A139:F139"/>
+    <mergeCell ref="A140:F140"/>
+    <mergeCell ref="A141:F141"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A143:F143"/>
+    <mergeCell ref="A144:F144"/>
+    <mergeCell ref="A127:F127"/>
+    <mergeCell ref="A128:F128"/>
+    <mergeCell ref="A129:F129"/>
+    <mergeCell ref="A130:F130"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A132:F132"/>
+    <mergeCell ref="A133:F133"/>
+    <mergeCell ref="A134:F134"/>
+    <mergeCell ref="A135:F135"/>
+    <mergeCell ref="A118:F118"/>
+    <mergeCell ref="A119:F119"/>
+    <mergeCell ref="A120:F120"/>
+    <mergeCell ref="A121:F121"/>
+    <mergeCell ref="A122:F122"/>
+    <mergeCell ref="A123:F123"/>
+    <mergeCell ref="A124:F124"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="A126:F126"/>
+    <mergeCell ref="A109:F109"/>
+    <mergeCell ref="A110:F110"/>
+    <mergeCell ref="A111:F111"/>
+    <mergeCell ref="A112:F112"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A114:F114"/>
+    <mergeCell ref="A115:F115"/>
+    <mergeCell ref="A116:F116"/>
+    <mergeCell ref="A117:F117"/>
+    <mergeCell ref="A100:F100"/>
+    <mergeCell ref="A101:F101"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A103:F103"/>
+    <mergeCell ref="A104:F104"/>
+    <mergeCell ref="A105:F105"/>
+    <mergeCell ref="A106:F106"/>
+    <mergeCell ref="A107:F107"/>
+    <mergeCell ref="A108:F108"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A92:F92"/>
+    <mergeCell ref="A93:F93"/>
+    <mergeCell ref="A94:F94"/>
+    <mergeCell ref="A95:F95"/>
+    <mergeCell ref="A96:F96"/>
+    <mergeCell ref="A97:F97"/>
+    <mergeCell ref="A98:F98"/>
+    <mergeCell ref="A99:F99"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A83:F83"/>
+    <mergeCell ref="A84:F84"/>
+    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="A86:F86"/>
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A88:F88"/>
+    <mergeCell ref="A89:F89"/>
+    <mergeCell ref="A90:F90"/>
+    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="A74:F74"/>
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="A76:F76"/>
+    <mergeCell ref="A77:F77"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A79:F79"/>
+    <mergeCell ref="A80:F80"/>
+    <mergeCell ref="A81:F81"/>
+    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="A71:F71"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A59:F59"/>
+    <mergeCell ref="A60:F60"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A49:F49"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>